<commit_message>
Polish rename function and directory in function description
</commit_message>
<xml_diff>
--- a/test_file/file_list.xlsx
+++ b/test_file/file_list.xlsx
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="E2">
-        <f>D2&amp;" """&amp;A2&amp;""" """&amp;C2&amp;B2</f>
+        <f>D2&amp;" """&amp;A2&amp;""" """&amp;C2&amp;B2&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="E3">
-        <f>D3&amp;" """&amp;A3&amp;""" """&amp;C3&amp;B3</f>
+        <f>D3&amp;" """&amp;A3&amp;""" """&amp;C3&amp;B3&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -534,7 +534,7 @@
         </is>
       </c>
       <c r="E4">
-        <f>D4&amp;" """&amp;A4&amp;""" """&amp;C4&amp;B4</f>
+        <f>D4&amp;" """&amp;A4&amp;""" """&amp;C4&amp;B4&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="E5">
-        <f>D5&amp;" """&amp;A5&amp;""" """&amp;C5&amp;B5</f>
+        <f>D5&amp;" """&amp;A5&amp;""" """&amp;C5&amp;B5&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="E6">
-        <f>D6&amp;" """&amp;A6&amp;""" """&amp;C6&amp;B6</f>
+        <f>D6&amp;" """&amp;A6&amp;""" """&amp;C6&amp;B6&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="E7">
-        <f>D7&amp;" """&amp;A7&amp;""" """&amp;C7&amp;B7</f>
+        <f>D7&amp;" """&amp;A7&amp;""" """&amp;C7&amp;B7&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -638,7 +638,7 @@
         </is>
       </c>
       <c r="E8">
-        <f>D8&amp;" """&amp;A8&amp;""" """&amp;C8&amp;B8</f>
+        <f>D8&amp;" """&amp;A8&amp;""" """&amp;C8&amp;B8&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -664,7 +664,7 @@
         </is>
       </c>
       <c r="E9">
-        <f>D9&amp;" """&amp;A9&amp;""" """&amp;C9&amp;B9</f>
+        <f>D9&amp;" """&amp;A9&amp;""" """&amp;C9&amp;B9&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="E10">
-        <f>D10&amp;" """&amp;A10&amp;""" """&amp;C10&amp;B10</f>
+        <f>D10&amp;" """&amp;A10&amp;""" """&amp;C10&amp;B10&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -716,7 +716,7 @@
         </is>
       </c>
       <c r="E11">
-        <f>D11&amp;" """&amp;A11&amp;""" """&amp;C11&amp;B11</f>
+        <f>D11&amp;" """&amp;A11&amp;""" """&amp;C11&amp;B11&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="E12">
-        <f>D12&amp;" """&amp;A12&amp;""" """&amp;C12&amp;B12</f>
+        <f>D12&amp;" """&amp;A12&amp;""" """&amp;C12&amp;B12&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -768,7 +768,7 @@
         </is>
       </c>
       <c r="E13">
-        <f>D13&amp;" """&amp;A13&amp;""" """&amp;C13&amp;B13</f>
+        <f>D13&amp;" """&amp;A13&amp;""" """&amp;C13&amp;B13&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -794,7 +794,7 @@
         </is>
       </c>
       <c r="E14">
-        <f>D14&amp;" """&amp;A14&amp;""" """&amp;C14&amp;B14</f>
+        <f>D14&amp;" """&amp;A14&amp;""" """&amp;C14&amp;B14&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -820,7 +820,7 @@
         </is>
       </c>
       <c r="E15">
-        <f>D15&amp;" """&amp;A15&amp;""" """&amp;C15&amp;B15</f>
+        <f>D15&amp;" """&amp;A15&amp;""" """&amp;C15&amp;B15&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -846,7 +846,7 @@
         </is>
       </c>
       <c r="E16">
-        <f>D16&amp;" """&amp;A16&amp;""" """&amp;C16&amp;B16</f>
+        <f>D16&amp;" """&amp;A16&amp;""" """&amp;C16&amp;B16&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="E17">
-        <f>D17&amp;" """&amp;A17&amp;""" """&amp;C17&amp;B17</f>
+        <f>D17&amp;" """&amp;A17&amp;""" """&amp;C17&amp;B17&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -898,7 +898,7 @@
         </is>
       </c>
       <c r="E18">
-        <f>D18&amp;" """&amp;A18&amp;""" """&amp;C18&amp;B18</f>
+        <f>D18&amp;" """&amp;A18&amp;""" """&amp;C18&amp;B18&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -924,7 +924,7 @@
         </is>
       </c>
       <c r="E19">
-        <f>D19&amp;" """&amp;A19&amp;""" """&amp;C19&amp;B19</f>
+        <f>D19&amp;" """&amp;A19&amp;""" """&amp;C19&amp;B19&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -950,7 +950,7 @@
         </is>
       </c>
       <c r="E20">
-        <f>D20&amp;" """&amp;A20&amp;""" """&amp;C20&amp;B20</f>
+        <f>D20&amp;" """&amp;A20&amp;""" """&amp;C20&amp;B20&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -976,7 +976,7 @@
         </is>
       </c>
       <c r="E21">
-        <f>D21&amp;" """&amp;A21&amp;""" """&amp;C21&amp;B21</f>
+        <f>D21&amp;" """&amp;A21&amp;""" """&amp;C21&amp;B21&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="E22">
-        <f>D22&amp;" """&amp;A22&amp;""" """&amp;C22&amp;B22</f>
+        <f>D22&amp;" """&amp;A22&amp;""" """&amp;C22&amp;B22&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
         </is>
       </c>
       <c r="E23">
-        <f>D23&amp;" """&amp;A23&amp;""" """&amp;C23&amp;B23</f>
+        <f>D23&amp;" """&amp;A23&amp;""" """&amp;C23&amp;B23&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1054,7 +1054,7 @@
         </is>
       </c>
       <c r="E24">
-        <f>D24&amp;" """&amp;A24&amp;""" """&amp;C24&amp;B24</f>
+        <f>D24&amp;" """&amp;A24&amp;""" """&amp;C24&amp;B24&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1080,7 +1080,7 @@
         </is>
       </c>
       <c r="E25">
-        <f>D25&amp;" """&amp;A25&amp;""" """&amp;C25&amp;B25</f>
+        <f>D25&amp;" """&amp;A25&amp;""" """&amp;C25&amp;B25&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1106,7 +1106,7 @@
         </is>
       </c>
       <c r="E26">
-        <f>D26&amp;" """&amp;A26&amp;""" """&amp;C26&amp;B26</f>
+        <f>D26&amp;" """&amp;A26&amp;""" """&amp;C26&amp;B26&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="E27">
-        <f>D27&amp;" """&amp;A27&amp;""" """&amp;C27&amp;B27</f>
+        <f>D27&amp;" """&amp;A27&amp;""" """&amp;C27&amp;B27&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1158,7 +1158,7 @@
         </is>
       </c>
       <c r="E28">
-        <f>D28&amp;" """&amp;A28&amp;""" """&amp;C28&amp;B28</f>
+        <f>D28&amp;" """&amp;A28&amp;""" """&amp;C28&amp;B28&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1184,7 +1184,7 @@
         </is>
       </c>
       <c r="E29">
-        <f>D29&amp;" """&amp;A29&amp;""" """&amp;C29&amp;B29</f>
+        <f>D29&amp;" """&amp;A29&amp;""" """&amp;C29&amp;B29&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1210,7 +1210,7 @@
         </is>
       </c>
       <c r="E30">
-        <f>D30&amp;" """&amp;A30&amp;""" """&amp;C30&amp;B30</f>
+        <f>D30&amp;" """&amp;A30&amp;""" """&amp;C30&amp;B30&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1236,7 +1236,7 @@
         </is>
       </c>
       <c r="E31">
-        <f>D31&amp;" """&amp;A31&amp;""" """&amp;C31&amp;B31</f>
+        <f>D31&amp;" """&amp;A31&amp;""" """&amp;C31&amp;B31&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="E32">
-        <f>D32&amp;" """&amp;A32&amp;""" """&amp;C32&amp;B32</f>
+        <f>D32&amp;" """&amp;A32&amp;""" """&amp;C32&amp;B32&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1288,7 +1288,7 @@
         </is>
       </c>
       <c r="E33">
-        <f>D33&amp;" """&amp;A33&amp;""" """&amp;C33&amp;B33</f>
+        <f>D33&amp;" """&amp;A33&amp;""" """&amp;C33&amp;B33&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1314,7 +1314,7 @@
         </is>
       </c>
       <c r="E34">
-        <f>D34&amp;" """&amp;A34&amp;""" """&amp;C34&amp;B34</f>
+        <f>D34&amp;" """&amp;A34&amp;""" """&amp;C34&amp;B34&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1340,7 +1340,7 @@
         </is>
       </c>
       <c r="E35">
-        <f>D35&amp;" """&amp;A35&amp;""" """&amp;C35&amp;B35</f>
+        <f>D35&amp;" """&amp;A35&amp;""" """&amp;C35&amp;B35&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1366,7 +1366,7 @@
         </is>
       </c>
       <c r="E36">
-        <f>D36&amp;" """&amp;A36&amp;""" """&amp;C36&amp;B36</f>
+        <f>D36&amp;" """&amp;A36&amp;""" """&amp;C36&amp;B36&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="E37">
-        <f>D37&amp;" """&amp;A37&amp;""" """&amp;C37&amp;B37</f>
+        <f>D37&amp;" """&amp;A37&amp;""" """&amp;C37&amp;B37&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1418,7 +1418,7 @@
         </is>
       </c>
       <c r="E38">
-        <f>D38&amp;" """&amp;A38&amp;""" """&amp;C38&amp;B38</f>
+        <f>D38&amp;" """&amp;A38&amp;""" """&amp;C38&amp;B38&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1444,7 +1444,7 @@
         </is>
       </c>
       <c r="E39">
-        <f>D39&amp;" """&amp;A39&amp;""" """&amp;C39&amp;B39</f>
+        <f>D39&amp;" """&amp;A39&amp;""" """&amp;C39&amp;B39&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1470,7 +1470,7 @@
         </is>
       </c>
       <c r="E40">
-        <f>D40&amp;" """&amp;A40&amp;""" """&amp;C40&amp;B40</f>
+        <f>D40&amp;" """&amp;A40&amp;""" """&amp;C40&amp;B40&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1496,7 +1496,7 @@
         </is>
       </c>
       <c r="E41">
-        <f>D41&amp;" """&amp;A41&amp;""" """&amp;C41&amp;B41</f>
+        <f>D41&amp;" """&amp;A41&amp;""" """&amp;C41&amp;B41&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1522,7 +1522,7 @@
         </is>
       </c>
       <c r="E42">
-        <f>D42&amp;" """&amp;A42&amp;""" """&amp;C42&amp;B42</f>
+        <f>D42&amp;" """&amp;A42&amp;""" """&amp;C42&amp;B42&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1548,7 +1548,7 @@
         </is>
       </c>
       <c r="E43">
-        <f>D43&amp;" """&amp;A43&amp;""" """&amp;C43&amp;B43</f>
+        <f>D43&amp;" """&amp;A43&amp;""" """&amp;C43&amp;B43&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1574,7 +1574,7 @@
         </is>
       </c>
       <c r="E44">
-        <f>D44&amp;" """&amp;A44&amp;""" """&amp;C44&amp;B44</f>
+        <f>D44&amp;" """&amp;A44&amp;""" """&amp;C44&amp;B44&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1600,7 +1600,7 @@
         </is>
       </c>
       <c r="E45">
-        <f>D45&amp;" """&amp;A45&amp;""" """&amp;C45&amp;B45</f>
+        <f>D45&amp;" """&amp;A45&amp;""" """&amp;C45&amp;B45&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1626,7 +1626,7 @@
         </is>
       </c>
       <c r="E46">
-        <f>D46&amp;" """&amp;A46&amp;""" """&amp;C46&amp;B46</f>
+        <f>D46&amp;" """&amp;A46&amp;""" """&amp;C46&amp;B46&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1652,7 +1652,7 @@
         </is>
       </c>
       <c r="E47">
-        <f>D47&amp;" """&amp;A47&amp;""" """&amp;C47&amp;B47</f>
+        <f>D47&amp;" """&amp;A47&amp;""" """&amp;C47&amp;B47&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1678,7 +1678,7 @@
         </is>
       </c>
       <c r="E48">
-        <f>D48&amp;" """&amp;A48&amp;""" """&amp;C48&amp;B48</f>
+        <f>D48&amp;" """&amp;A48&amp;""" """&amp;C48&amp;B48&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1704,7 +1704,7 @@
         </is>
       </c>
       <c r="E49">
-        <f>D49&amp;" """&amp;A49&amp;""" """&amp;C49&amp;B49</f>
+        <f>D49&amp;" """&amp;A49&amp;""" """&amp;C49&amp;B49&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1730,7 +1730,7 @@
         </is>
       </c>
       <c r="E50">
-        <f>D50&amp;" """&amp;A50&amp;""" """&amp;C50&amp;B50</f>
+        <f>D50&amp;" """&amp;A50&amp;""" """&amp;C50&amp;B50&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1756,7 +1756,7 @@
         </is>
       </c>
       <c r="E51">
-        <f>D51&amp;" """&amp;A51&amp;""" """&amp;C51&amp;B51</f>
+        <f>D51&amp;" """&amp;A51&amp;""" """&amp;C51&amp;B51&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="E52">
-        <f>D52&amp;" """&amp;A52&amp;""" """&amp;C52&amp;B52</f>
+        <f>D52&amp;" """&amp;A52&amp;""" """&amp;C52&amp;B52&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1808,7 +1808,7 @@
         </is>
       </c>
       <c r="E53">
-        <f>D53&amp;" """&amp;A53&amp;""" """&amp;C53&amp;B53</f>
+        <f>D53&amp;" """&amp;A53&amp;""" """&amp;C53&amp;B53&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1834,7 +1834,7 @@
         </is>
       </c>
       <c r="E54">
-        <f>D54&amp;" """&amp;A54&amp;""" """&amp;C54&amp;B54</f>
+        <f>D54&amp;" """&amp;A54&amp;""" """&amp;C54&amp;B54&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1860,7 +1860,7 @@
         </is>
       </c>
       <c r="E55">
-        <f>D55&amp;" """&amp;A55&amp;""" """&amp;C55&amp;B55</f>
+        <f>D55&amp;" """&amp;A55&amp;""" """&amp;C55&amp;B55&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1886,7 +1886,7 @@
         </is>
       </c>
       <c r="E56">
-        <f>D56&amp;" """&amp;A56&amp;""" """&amp;C56&amp;B56</f>
+        <f>D56&amp;" """&amp;A56&amp;""" """&amp;C56&amp;B56&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1912,7 +1912,7 @@
         </is>
       </c>
       <c r="E57">
-        <f>D57&amp;" """&amp;A57&amp;""" """&amp;C57&amp;B57</f>
+        <f>D57&amp;" """&amp;A57&amp;""" """&amp;C57&amp;B57&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1938,7 +1938,7 @@
         </is>
       </c>
       <c r="E58">
-        <f>D58&amp;" """&amp;A58&amp;""" """&amp;C58&amp;B58</f>
+        <f>D58&amp;" """&amp;A58&amp;""" """&amp;C58&amp;B58&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1964,7 +1964,7 @@
         </is>
       </c>
       <c r="E59">
-        <f>D59&amp;" """&amp;A59&amp;""" """&amp;C59&amp;B59</f>
+        <f>D59&amp;" """&amp;A59&amp;""" """&amp;C59&amp;B59&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -1990,7 +1990,7 @@
         </is>
       </c>
       <c r="E60">
-        <f>D60&amp;" """&amp;A60&amp;""" """&amp;C60&amp;B60</f>
+        <f>D60&amp;" """&amp;A60&amp;""" """&amp;C60&amp;B60&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2016,7 +2016,7 @@
         </is>
       </c>
       <c r="E61">
-        <f>D61&amp;" """&amp;A61&amp;""" """&amp;C61&amp;B61</f>
+        <f>D61&amp;" """&amp;A61&amp;""" """&amp;C61&amp;B61&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2042,7 +2042,7 @@
         </is>
       </c>
       <c r="E62">
-        <f>D62&amp;" """&amp;A62&amp;""" """&amp;C62&amp;B62</f>
+        <f>D62&amp;" """&amp;A62&amp;""" """&amp;C62&amp;B62&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2068,7 +2068,7 @@
         </is>
       </c>
       <c r="E63">
-        <f>D63&amp;" """&amp;A63&amp;""" """&amp;C63&amp;B63</f>
+        <f>D63&amp;" """&amp;A63&amp;""" """&amp;C63&amp;B63&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2094,7 +2094,7 @@
         </is>
       </c>
       <c r="E64">
-        <f>D64&amp;" """&amp;A64&amp;""" """&amp;C64&amp;B64</f>
+        <f>D64&amp;" """&amp;A64&amp;""" """&amp;C64&amp;B64&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2120,7 +2120,7 @@
         </is>
       </c>
       <c r="E65">
-        <f>D65&amp;" """&amp;A65&amp;""" """&amp;C65&amp;B65</f>
+        <f>D65&amp;" """&amp;A65&amp;""" """&amp;C65&amp;B65&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2146,7 +2146,7 @@
         </is>
       </c>
       <c r="E66">
-        <f>D66&amp;" """&amp;A66&amp;""" """&amp;C66&amp;B66</f>
+        <f>D66&amp;" """&amp;A66&amp;""" """&amp;C66&amp;B66&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2172,7 +2172,7 @@
         </is>
       </c>
       <c r="E67">
-        <f>D67&amp;" """&amp;A67&amp;""" """&amp;C67&amp;B67</f>
+        <f>D67&amp;" """&amp;A67&amp;""" """&amp;C67&amp;B67&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
         </is>
       </c>
       <c r="E68">
-        <f>D68&amp;" """&amp;A68&amp;""" """&amp;C68&amp;B68</f>
+        <f>D68&amp;" """&amp;A68&amp;""" """&amp;C68&amp;B68&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2224,7 +2224,7 @@
         </is>
       </c>
       <c r="E69">
-        <f>D69&amp;" """&amp;A69&amp;""" """&amp;C69&amp;B69</f>
+        <f>D69&amp;" """&amp;A69&amp;""" """&amp;C69&amp;B69&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2250,7 +2250,7 @@
         </is>
       </c>
       <c r="E70">
-        <f>D70&amp;" """&amp;A70&amp;""" """&amp;C70&amp;B70</f>
+        <f>D70&amp;" """&amp;A70&amp;""" """&amp;C70&amp;B70&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2276,7 +2276,7 @@
         </is>
       </c>
       <c r="E71">
-        <f>D71&amp;" """&amp;A71&amp;""" """&amp;C71&amp;B71</f>
+        <f>D71&amp;" """&amp;A71&amp;""" """&amp;C71&amp;B71&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2302,7 +2302,7 @@
         </is>
       </c>
       <c r="E72">
-        <f>D72&amp;" """&amp;A72&amp;""" """&amp;C72&amp;B72</f>
+        <f>D72&amp;" """&amp;A72&amp;""" """&amp;C72&amp;B72&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2328,7 +2328,7 @@
         </is>
       </c>
       <c r="E73">
-        <f>D73&amp;" """&amp;A73&amp;""" """&amp;C73&amp;B73</f>
+        <f>D73&amp;" """&amp;A73&amp;""" """&amp;C73&amp;B73&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2354,7 +2354,7 @@
         </is>
       </c>
       <c r="E74">
-        <f>D74&amp;" """&amp;A74&amp;""" """&amp;C74&amp;B74</f>
+        <f>D74&amp;" """&amp;A74&amp;""" """&amp;C74&amp;B74&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2380,7 +2380,7 @@
         </is>
       </c>
       <c r="E75">
-        <f>D75&amp;" """&amp;A75&amp;""" """&amp;C75&amp;B75</f>
+        <f>D75&amp;" """&amp;A75&amp;""" """&amp;C75&amp;B75&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2406,7 +2406,7 @@
         </is>
       </c>
       <c r="E76">
-        <f>D76&amp;" """&amp;A76&amp;""" """&amp;C76&amp;B76</f>
+        <f>D76&amp;" """&amp;A76&amp;""" """&amp;C76&amp;B76&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2432,7 +2432,7 @@
         </is>
       </c>
       <c r="E77">
-        <f>D77&amp;" """&amp;A77&amp;""" """&amp;C77&amp;B77</f>
+        <f>D77&amp;" """&amp;A77&amp;""" """&amp;C77&amp;B77&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2458,7 +2458,7 @@
         </is>
       </c>
       <c r="E78">
-        <f>D78&amp;" """&amp;A78&amp;""" """&amp;C78&amp;B78</f>
+        <f>D78&amp;" """&amp;A78&amp;""" """&amp;C78&amp;B78&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2484,7 +2484,7 @@
         </is>
       </c>
       <c r="E79">
-        <f>D79&amp;" """&amp;A79&amp;""" """&amp;C79&amp;B79</f>
+        <f>D79&amp;" """&amp;A79&amp;""" """&amp;C79&amp;B79&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2510,7 +2510,7 @@
         </is>
       </c>
       <c r="E80">
-        <f>D80&amp;" """&amp;A80&amp;""" """&amp;C80&amp;B80</f>
+        <f>D80&amp;" """&amp;A80&amp;""" """&amp;C80&amp;B80&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2536,7 +2536,7 @@
         </is>
       </c>
       <c r="E81">
-        <f>D81&amp;" """&amp;A81&amp;""" """&amp;C81&amp;B81</f>
+        <f>D81&amp;" """&amp;A81&amp;""" """&amp;C81&amp;B81&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2562,7 +2562,7 @@
         </is>
       </c>
       <c r="E82">
-        <f>D82&amp;" """&amp;A82&amp;""" """&amp;C82&amp;B82</f>
+        <f>D82&amp;" """&amp;A82&amp;""" """&amp;C82&amp;B82&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2588,7 +2588,7 @@
         </is>
       </c>
       <c r="E83">
-        <f>D83&amp;" """&amp;A83&amp;""" """&amp;C83&amp;B83</f>
+        <f>D83&amp;" """&amp;A83&amp;""" """&amp;C83&amp;B83&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2614,7 +2614,7 @@
         </is>
       </c>
       <c r="E84">
-        <f>D84&amp;" """&amp;A84&amp;""" """&amp;C84&amp;B84</f>
+        <f>D84&amp;" """&amp;A84&amp;""" """&amp;C84&amp;B84&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2640,7 +2640,7 @@
         </is>
       </c>
       <c r="E85">
-        <f>D85&amp;" """&amp;A85&amp;""" """&amp;C85&amp;B85</f>
+        <f>D85&amp;" """&amp;A85&amp;""" """&amp;C85&amp;B85&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2666,7 +2666,7 @@
         </is>
       </c>
       <c r="E86">
-        <f>D86&amp;" """&amp;A86&amp;""" """&amp;C86&amp;B86</f>
+        <f>D86&amp;" """&amp;A86&amp;""" """&amp;C86&amp;B86&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2692,7 +2692,7 @@
         </is>
       </c>
       <c r="E87">
-        <f>D87&amp;" """&amp;A87&amp;""" """&amp;C87&amp;B87</f>
+        <f>D87&amp;" """&amp;A87&amp;""" """&amp;C87&amp;B87&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2718,7 +2718,7 @@
         </is>
       </c>
       <c r="E88">
-        <f>D88&amp;" """&amp;A88&amp;""" """&amp;C88&amp;B88</f>
+        <f>D88&amp;" """&amp;A88&amp;""" """&amp;C88&amp;B88&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2744,7 +2744,7 @@
         </is>
       </c>
       <c r="E89">
-        <f>D89&amp;" """&amp;A89&amp;""" """&amp;C89&amp;B89</f>
+        <f>D89&amp;" """&amp;A89&amp;""" """&amp;C89&amp;B89&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2770,7 +2770,7 @@
         </is>
       </c>
       <c r="E90">
-        <f>D90&amp;" """&amp;A90&amp;""" """&amp;C90&amp;B90</f>
+        <f>D90&amp;" """&amp;A90&amp;""" """&amp;C90&amp;B90&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2796,7 +2796,7 @@
         </is>
       </c>
       <c r="E91">
-        <f>D91&amp;" """&amp;A91&amp;""" """&amp;C91&amp;B91</f>
+        <f>D91&amp;" """&amp;A91&amp;""" """&amp;C91&amp;B91&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2822,7 +2822,7 @@
         </is>
       </c>
       <c r="E92">
-        <f>D92&amp;" """&amp;A92&amp;""" """&amp;C92&amp;B92</f>
+        <f>D92&amp;" """&amp;A92&amp;""" """&amp;C92&amp;B92&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2848,7 +2848,7 @@
         </is>
       </c>
       <c r="E93">
-        <f>D93&amp;" """&amp;A93&amp;""" """&amp;C93&amp;B93</f>
+        <f>D93&amp;" """&amp;A93&amp;""" """&amp;C93&amp;B93&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2874,7 +2874,7 @@
         </is>
       </c>
       <c r="E94">
-        <f>D94&amp;" """&amp;A94&amp;""" """&amp;C94&amp;B94</f>
+        <f>D94&amp;" """&amp;A94&amp;""" """&amp;C94&amp;B94&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2900,7 +2900,7 @@
         </is>
       </c>
       <c r="E95">
-        <f>D95&amp;" """&amp;A95&amp;""" """&amp;C95&amp;B95</f>
+        <f>D95&amp;" """&amp;A95&amp;""" """&amp;C95&amp;B95&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2926,7 +2926,7 @@
         </is>
       </c>
       <c r="E96">
-        <f>D96&amp;" """&amp;A96&amp;""" """&amp;C96&amp;B96</f>
+        <f>D96&amp;" """&amp;A96&amp;""" """&amp;C96&amp;B96&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2952,7 +2952,7 @@
         </is>
       </c>
       <c r="E97">
-        <f>D97&amp;" """&amp;A97&amp;""" """&amp;C97&amp;B97</f>
+        <f>D97&amp;" """&amp;A97&amp;""" """&amp;C97&amp;B97&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -2978,7 +2978,7 @@
         </is>
       </c>
       <c r="E98">
-        <f>D98&amp;" """&amp;A98&amp;""" """&amp;C98&amp;B98</f>
+        <f>D98&amp;" """&amp;A98&amp;""" """&amp;C98&amp;B98&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3004,7 +3004,7 @@
         </is>
       </c>
       <c r="E99">
-        <f>D99&amp;" """&amp;A99&amp;""" """&amp;C99&amp;B99</f>
+        <f>D99&amp;" """&amp;A99&amp;""" """&amp;C99&amp;B99&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3030,7 +3030,7 @@
         </is>
       </c>
       <c r="E100">
-        <f>D100&amp;" """&amp;A100&amp;""" """&amp;C100&amp;B100</f>
+        <f>D100&amp;" """&amp;A100&amp;""" """&amp;C100&amp;B100&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3056,7 +3056,7 @@
         </is>
       </c>
       <c r="E101">
-        <f>D101&amp;" """&amp;A101&amp;""" """&amp;C101&amp;B101</f>
+        <f>D101&amp;" """&amp;A101&amp;""" """&amp;C101&amp;B101&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3082,7 +3082,7 @@
         </is>
       </c>
       <c r="E102">
-        <f>D102&amp;" """&amp;A102&amp;""" """&amp;C102&amp;B102</f>
+        <f>D102&amp;" """&amp;A102&amp;""" """&amp;C102&amp;B102&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3108,7 +3108,7 @@
         </is>
       </c>
       <c r="E103">
-        <f>D103&amp;" """&amp;A103&amp;""" """&amp;C103&amp;B103</f>
+        <f>D103&amp;" """&amp;A103&amp;""" """&amp;C103&amp;B103&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3134,7 +3134,7 @@
         </is>
       </c>
       <c r="E104">
-        <f>D104&amp;" """&amp;A104&amp;""" """&amp;C104&amp;B104</f>
+        <f>D104&amp;" """&amp;A104&amp;""" """&amp;C104&amp;B104&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3160,7 +3160,7 @@
         </is>
       </c>
       <c r="E105">
-        <f>D105&amp;" """&amp;A105&amp;""" """&amp;C105&amp;B105</f>
+        <f>D105&amp;" """&amp;A105&amp;""" """&amp;C105&amp;B105&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3186,7 +3186,7 @@
         </is>
       </c>
       <c r="E106">
-        <f>D106&amp;" """&amp;A106&amp;""" """&amp;C106&amp;B106</f>
+        <f>D106&amp;" """&amp;A106&amp;""" """&amp;C106&amp;B106&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3212,7 +3212,7 @@
         </is>
       </c>
       <c r="E107">
-        <f>D107&amp;" """&amp;A107&amp;""" """&amp;C107&amp;B107</f>
+        <f>D107&amp;" """&amp;A107&amp;""" """&amp;C107&amp;B107&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3238,7 +3238,7 @@
         </is>
       </c>
       <c r="E108">
-        <f>D108&amp;" """&amp;A108&amp;""" """&amp;C108&amp;B108</f>
+        <f>D108&amp;" """&amp;A108&amp;""" """&amp;C108&amp;B108&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3264,7 +3264,7 @@
         </is>
       </c>
       <c r="E109">
-        <f>D109&amp;" """&amp;A109&amp;""" """&amp;C109&amp;B109</f>
+        <f>D109&amp;" """&amp;A109&amp;""" """&amp;C109&amp;B109&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3290,7 +3290,7 @@
         </is>
       </c>
       <c r="E110">
-        <f>D110&amp;" """&amp;A110&amp;""" """&amp;C110&amp;B110</f>
+        <f>D110&amp;" """&amp;A110&amp;""" """&amp;C110&amp;B110&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3316,7 +3316,7 @@
         </is>
       </c>
       <c r="E111">
-        <f>D111&amp;" """&amp;A111&amp;""" """&amp;C111&amp;B111</f>
+        <f>D111&amp;" """&amp;A111&amp;""" """&amp;C111&amp;B111&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3342,7 +3342,7 @@
         </is>
       </c>
       <c r="E112">
-        <f>D112&amp;" """&amp;A112&amp;""" """&amp;C112&amp;B112</f>
+        <f>D112&amp;" """&amp;A112&amp;""" """&amp;C112&amp;B112&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3368,7 +3368,7 @@
         </is>
       </c>
       <c r="E113">
-        <f>D113&amp;" """&amp;A113&amp;""" """&amp;C113&amp;B113</f>
+        <f>D113&amp;" """&amp;A113&amp;""" """&amp;C113&amp;B113&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3394,7 +3394,7 @@
         </is>
       </c>
       <c r="E114">
-        <f>D114&amp;" """&amp;A114&amp;""" """&amp;C114&amp;B114</f>
+        <f>D114&amp;" """&amp;A114&amp;""" """&amp;C114&amp;B114&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3420,7 +3420,7 @@
         </is>
       </c>
       <c r="E115">
-        <f>D115&amp;" """&amp;A115&amp;""" """&amp;C115&amp;B115</f>
+        <f>D115&amp;" """&amp;A115&amp;""" """&amp;C115&amp;B115&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3446,7 +3446,7 @@
         </is>
       </c>
       <c r="E116">
-        <f>D116&amp;" """&amp;A116&amp;""" """&amp;C116&amp;B116</f>
+        <f>D116&amp;" """&amp;A116&amp;""" """&amp;C116&amp;B116&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3472,7 +3472,7 @@
         </is>
       </c>
       <c r="E117">
-        <f>D117&amp;" """&amp;A117&amp;""" """&amp;C117&amp;B117</f>
+        <f>D117&amp;" """&amp;A117&amp;""" """&amp;C117&amp;B117&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3498,7 +3498,7 @@
         </is>
       </c>
       <c r="E118">
-        <f>D118&amp;" """&amp;A118&amp;""" """&amp;C118&amp;B118</f>
+        <f>D118&amp;" """&amp;A118&amp;""" """&amp;C118&amp;B118&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3524,7 +3524,7 @@
         </is>
       </c>
       <c r="E119">
-        <f>D119&amp;" """&amp;A119&amp;""" """&amp;C119&amp;B119</f>
+        <f>D119&amp;" """&amp;A119&amp;""" """&amp;C119&amp;B119&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3550,7 +3550,7 @@
         </is>
       </c>
       <c r="E120">
-        <f>D120&amp;" """&amp;A120&amp;""" """&amp;C120&amp;B120</f>
+        <f>D120&amp;" """&amp;A120&amp;""" """&amp;C120&amp;B120&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3576,7 +3576,7 @@
         </is>
       </c>
       <c r="E121">
-        <f>D121&amp;" """&amp;A121&amp;""" """&amp;C121&amp;B121</f>
+        <f>D121&amp;" """&amp;A121&amp;""" """&amp;C121&amp;B121&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3602,7 +3602,7 @@
         </is>
       </c>
       <c r="E122">
-        <f>D122&amp;" """&amp;A122&amp;""" """&amp;C122&amp;B122</f>
+        <f>D122&amp;" """&amp;A122&amp;""" """&amp;C122&amp;B122&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3628,7 +3628,7 @@
         </is>
       </c>
       <c r="E123">
-        <f>D123&amp;" """&amp;A123&amp;""" """&amp;C123&amp;B123</f>
+        <f>D123&amp;" """&amp;A123&amp;""" """&amp;C123&amp;B123&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3654,7 +3654,7 @@
         </is>
       </c>
       <c r="E124">
-        <f>D124&amp;" """&amp;A124&amp;""" """&amp;C124&amp;B124</f>
+        <f>D124&amp;" """&amp;A124&amp;""" """&amp;C124&amp;B124&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3680,7 +3680,7 @@
         </is>
       </c>
       <c r="E125">
-        <f>D125&amp;" """&amp;A125&amp;""" """&amp;C125&amp;B125</f>
+        <f>D125&amp;" """&amp;A125&amp;""" """&amp;C125&amp;B125&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3706,7 +3706,7 @@
         </is>
       </c>
       <c r="E126">
-        <f>D126&amp;" """&amp;A126&amp;""" """&amp;C126&amp;B126</f>
+        <f>D126&amp;" """&amp;A126&amp;""" """&amp;C126&amp;B126&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3732,7 +3732,7 @@
         </is>
       </c>
       <c r="E127">
-        <f>D127&amp;" """&amp;A127&amp;""" """&amp;C127&amp;B127</f>
+        <f>D127&amp;" """&amp;A127&amp;""" """&amp;C127&amp;B127&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3758,7 +3758,7 @@
         </is>
       </c>
       <c r="E128">
-        <f>D128&amp;" """&amp;A128&amp;""" """&amp;C128&amp;B128</f>
+        <f>D128&amp;" """&amp;A128&amp;""" """&amp;C128&amp;B128&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3784,7 +3784,7 @@
         </is>
       </c>
       <c r="E129">
-        <f>D129&amp;" """&amp;A129&amp;""" """&amp;C129&amp;B129</f>
+        <f>D129&amp;" """&amp;A129&amp;""" """&amp;C129&amp;B129&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3810,7 +3810,7 @@
         </is>
       </c>
       <c r="E130">
-        <f>D130&amp;" """&amp;A130&amp;""" """&amp;C130&amp;B130</f>
+        <f>D130&amp;" """&amp;A130&amp;""" """&amp;C130&amp;B130&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3836,7 +3836,7 @@
         </is>
       </c>
       <c r="E131">
-        <f>D131&amp;" """&amp;A131&amp;""" """&amp;C131&amp;B131</f>
+        <f>D131&amp;" """&amp;A131&amp;""" """&amp;C131&amp;B131&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3862,7 +3862,7 @@
         </is>
       </c>
       <c r="E132">
-        <f>D132&amp;" """&amp;A132&amp;""" """&amp;C132&amp;B132</f>
+        <f>D132&amp;" """&amp;A132&amp;""" """&amp;C132&amp;B132&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3888,7 +3888,7 @@
         </is>
       </c>
       <c r="E133">
-        <f>D133&amp;" """&amp;A133&amp;""" """&amp;C133&amp;B133</f>
+        <f>D133&amp;" """&amp;A133&amp;""" """&amp;C133&amp;B133&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3914,7 +3914,7 @@
         </is>
       </c>
       <c r="E134">
-        <f>D134&amp;" """&amp;A134&amp;""" """&amp;C134&amp;B134</f>
+        <f>D134&amp;" """&amp;A134&amp;""" """&amp;C134&amp;B134&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3940,7 +3940,7 @@
         </is>
       </c>
       <c r="E135">
-        <f>D135&amp;" """&amp;A135&amp;""" """&amp;C135&amp;B135</f>
+        <f>D135&amp;" """&amp;A135&amp;""" """&amp;C135&amp;B135&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3966,7 +3966,7 @@
         </is>
       </c>
       <c r="E136">
-        <f>D136&amp;" """&amp;A136&amp;""" """&amp;C136&amp;B136</f>
+        <f>D136&amp;" """&amp;A136&amp;""" """&amp;C136&amp;B136&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -3992,7 +3992,7 @@
         </is>
       </c>
       <c r="E137">
-        <f>D137&amp;" """&amp;A137&amp;""" """&amp;C137&amp;B137</f>
+        <f>D137&amp;" """&amp;A137&amp;""" """&amp;C137&amp;B137&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4018,7 +4018,7 @@
         </is>
       </c>
       <c r="E138">
-        <f>D138&amp;" """&amp;A138&amp;""" """&amp;C138&amp;B138</f>
+        <f>D138&amp;" """&amp;A138&amp;""" """&amp;C138&amp;B138&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4044,7 +4044,7 @@
         </is>
       </c>
       <c r="E139">
-        <f>D139&amp;" """&amp;A139&amp;""" """&amp;C139&amp;B139</f>
+        <f>D139&amp;" """&amp;A139&amp;""" """&amp;C139&amp;B139&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4070,7 +4070,7 @@
         </is>
       </c>
       <c r="E140">
-        <f>D140&amp;" """&amp;A140&amp;""" """&amp;C140&amp;B140</f>
+        <f>D140&amp;" """&amp;A140&amp;""" """&amp;C140&amp;B140&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4096,7 +4096,7 @@
         </is>
       </c>
       <c r="E141">
-        <f>D141&amp;" """&amp;A141&amp;""" """&amp;C141&amp;B141</f>
+        <f>D141&amp;" """&amp;A141&amp;""" """&amp;C141&amp;B141&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4122,7 +4122,7 @@
         </is>
       </c>
       <c r="E142">
-        <f>D142&amp;" """&amp;A142&amp;""" """&amp;C142&amp;B142</f>
+        <f>D142&amp;" """&amp;A142&amp;""" """&amp;C142&amp;B142&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4148,7 +4148,7 @@
         </is>
       </c>
       <c r="E143">
-        <f>D143&amp;" """&amp;A143&amp;""" """&amp;C143&amp;B143</f>
+        <f>D143&amp;" """&amp;A143&amp;""" """&amp;C143&amp;B143&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4174,7 +4174,7 @@
         </is>
       </c>
       <c r="E144">
-        <f>D144&amp;" """&amp;A144&amp;""" """&amp;C144&amp;B144</f>
+        <f>D144&amp;" """&amp;A144&amp;""" """&amp;C144&amp;B144&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4200,7 +4200,7 @@
         </is>
       </c>
       <c r="E145">
-        <f>D145&amp;" """&amp;A145&amp;""" """&amp;C145&amp;B145</f>
+        <f>D145&amp;" """&amp;A145&amp;""" """&amp;C145&amp;B145&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4226,7 +4226,7 @@
         </is>
       </c>
       <c r="E146">
-        <f>D146&amp;" """&amp;A146&amp;""" """&amp;C146&amp;B146</f>
+        <f>D146&amp;" """&amp;A146&amp;""" """&amp;C146&amp;B146&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4252,7 +4252,7 @@
         </is>
       </c>
       <c r="E147">
-        <f>D147&amp;" """&amp;A147&amp;""" """&amp;C147&amp;B147</f>
+        <f>D147&amp;" """&amp;A147&amp;""" """&amp;C147&amp;B147&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4278,7 +4278,7 @@
         </is>
       </c>
       <c r="E148">
-        <f>D148&amp;" """&amp;A148&amp;""" """&amp;C148&amp;B148</f>
+        <f>D148&amp;" """&amp;A148&amp;""" """&amp;C148&amp;B148&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4304,7 +4304,7 @@
         </is>
       </c>
       <c r="E149">
-        <f>D149&amp;" """&amp;A149&amp;""" """&amp;C149&amp;B149</f>
+        <f>D149&amp;" """&amp;A149&amp;""" """&amp;C149&amp;B149&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="E150">
-        <f>D150&amp;" """&amp;A150&amp;""" """&amp;C150&amp;B150</f>
+        <f>D150&amp;" """&amp;A150&amp;""" """&amp;C150&amp;B150&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4356,7 +4356,7 @@
         </is>
       </c>
       <c r="E151">
-        <f>D151&amp;" """&amp;A151&amp;""" """&amp;C151&amp;B151</f>
+        <f>D151&amp;" """&amp;A151&amp;""" """&amp;C151&amp;B151&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4382,7 +4382,7 @@
         </is>
       </c>
       <c r="E152">
-        <f>D152&amp;" """&amp;A152&amp;""" """&amp;C152&amp;B152</f>
+        <f>D152&amp;" """&amp;A152&amp;""" """&amp;C152&amp;B152&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4408,7 +4408,7 @@
         </is>
       </c>
       <c r="E153">
-        <f>D153&amp;" """&amp;A153&amp;""" """&amp;C153&amp;B153</f>
+        <f>D153&amp;" """&amp;A153&amp;""" """&amp;C153&amp;B153&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4434,7 +4434,7 @@
         </is>
       </c>
       <c r="E154">
-        <f>D154&amp;" """&amp;A154&amp;""" """&amp;C154&amp;B154</f>
+        <f>D154&amp;" """&amp;A154&amp;""" """&amp;C154&amp;B154&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4460,7 +4460,7 @@
         </is>
       </c>
       <c r="E155">
-        <f>D155&amp;" """&amp;A155&amp;""" """&amp;C155&amp;B155</f>
+        <f>D155&amp;" """&amp;A155&amp;""" """&amp;C155&amp;B155&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4486,7 +4486,7 @@
         </is>
       </c>
       <c r="E156">
-        <f>D156&amp;" """&amp;A156&amp;""" """&amp;C156&amp;B156</f>
+        <f>D156&amp;" """&amp;A156&amp;""" """&amp;C156&amp;B156&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4512,7 +4512,7 @@
         </is>
       </c>
       <c r="E157">
-        <f>D157&amp;" """&amp;A157&amp;""" """&amp;C157&amp;B157</f>
+        <f>D157&amp;" """&amp;A157&amp;""" """&amp;C157&amp;B157&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4538,7 +4538,7 @@
         </is>
       </c>
       <c r="E158">
-        <f>D158&amp;" """&amp;A158&amp;""" """&amp;C158&amp;B158</f>
+        <f>D158&amp;" """&amp;A158&amp;""" """&amp;C158&amp;B158&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4564,7 +4564,7 @@
         </is>
       </c>
       <c r="E159">
-        <f>D159&amp;" """&amp;A159&amp;""" """&amp;C159&amp;B159</f>
+        <f>D159&amp;" """&amp;A159&amp;""" """&amp;C159&amp;B159&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4590,7 +4590,7 @@
         </is>
       </c>
       <c r="E160">
-        <f>D160&amp;" """&amp;A160&amp;""" """&amp;C160&amp;B160</f>
+        <f>D160&amp;" """&amp;A160&amp;""" """&amp;C160&amp;B160&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4616,7 +4616,7 @@
         </is>
       </c>
       <c r="E161">
-        <f>D161&amp;" """&amp;A161&amp;""" """&amp;C161&amp;B161</f>
+        <f>D161&amp;" """&amp;A161&amp;""" """&amp;C161&amp;B161&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4642,7 +4642,7 @@
         </is>
       </c>
       <c r="E162">
-        <f>D162&amp;" """&amp;A162&amp;""" """&amp;C162&amp;B162</f>
+        <f>D162&amp;" """&amp;A162&amp;""" """&amp;C162&amp;B162&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4668,7 +4668,7 @@
         </is>
       </c>
       <c r="E163">
-        <f>D163&amp;" """&amp;A163&amp;""" """&amp;C163&amp;B163</f>
+        <f>D163&amp;" """&amp;A163&amp;""" """&amp;C163&amp;B163&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4694,7 +4694,7 @@
         </is>
       </c>
       <c r="E164">
-        <f>D164&amp;" """&amp;A164&amp;""" """&amp;C164&amp;B164</f>
+        <f>D164&amp;" """&amp;A164&amp;""" """&amp;C164&amp;B164&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4720,7 +4720,7 @@
         </is>
       </c>
       <c r="E165">
-        <f>D165&amp;" """&amp;A165&amp;""" """&amp;C165&amp;B165</f>
+        <f>D165&amp;" """&amp;A165&amp;""" """&amp;C165&amp;B165&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4746,7 +4746,7 @@
         </is>
       </c>
       <c r="E166">
-        <f>D166&amp;" """&amp;A166&amp;""" """&amp;C166&amp;B166</f>
+        <f>D166&amp;" """&amp;A166&amp;""" """&amp;C166&amp;B166&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4772,7 +4772,7 @@
         </is>
       </c>
       <c r="E167">
-        <f>D167&amp;" """&amp;A167&amp;""" """&amp;C167&amp;B167</f>
+        <f>D167&amp;" """&amp;A167&amp;""" """&amp;C167&amp;B167&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4798,7 +4798,7 @@
         </is>
       </c>
       <c r="E168">
-        <f>D168&amp;" """&amp;A168&amp;""" """&amp;C168&amp;B168</f>
+        <f>D168&amp;" """&amp;A168&amp;""" """&amp;C168&amp;B168&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4824,7 +4824,7 @@
         </is>
       </c>
       <c r="E169">
-        <f>D169&amp;" """&amp;A169&amp;""" """&amp;C169&amp;B169</f>
+        <f>D169&amp;" """&amp;A169&amp;""" """&amp;C169&amp;B169&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4850,7 +4850,7 @@
         </is>
       </c>
       <c r="E170">
-        <f>D170&amp;" """&amp;A170&amp;""" """&amp;C170&amp;B170</f>
+        <f>D170&amp;" """&amp;A170&amp;""" """&amp;C170&amp;B170&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4876,7 +4876,7 @@
         </is>
       </c>
       <c r="E171">
-        <f>D171&amp;" """&amp;A171&amp;""" """&amp;C171&amp;B171</f>
+        <f>D171&amp;" """&amp;A171&amp;""" """&amp;C171&amp;B171&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4902,7 +4902,7 @@
         </is>
       </c>
       <c r="E172">
-        <f>D172&amp;" """&amp;A172&amp;""" """&amp;C172&amp;B172</f>
+        <f>D172&amp;" """&amp;A172&amp;""" """&amp;C172&amp;B172&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4928,7 +4928,7 @@
         </is>
       </c>
       <c r="E173">
-        <f>D173&amp;" """&amp;A173&amp;""" """&amp;C173&amp;B173</f>
+        <f>D173&amp;" """&amp;A173&amp;""" """&amp;C173&amp;B173&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4954,7 +4954,7 @@
         </is>
       </c>
       <c r="E174">
-        <f>D174&amp;" """&amp;A174&amp;""" """&amp;C174&amp;B174</f>
+        <f>D174&amp;" """&amp;A174&amp;""" """&amp;C174&amp;B174&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -4980,7 +4980,7 @@
         </is>
       </c>
       <c r="E175">
-        <f>D175&amp;" """&amp;A175&amp;""" """&amp;C175&amp;B175</f>
+        <f>D175&amp;" """&amp;A175&amp;""" """&amp;C175&amp;B175&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5006,7 +5006,7 @@
         </is>
       </c>
       <c r="E176">
-        <f>D176&amp;" """&amp;A176&amp;""" """&amp;C176&amp;B176</f>
+        <f>D176&amp;" """&amp;A176&amp;""" """&amp;C176&amp;B176&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5032,7 +5032,7 @@
         </is>
       </c>
       <c r="E177">
-        <f>D177&amp;" """&amp;A177&amp;""" """&amp;C177&amp;B177</f>
+        <f>D177&amp;" """&amp;A177&amp;""" """&amp;C177&amp;B177&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5058,7 +5058,7 @@
         </is>
       </c>
       <c r="E178">
-        <f>D178&amp;" """&amp;A178&amp;""" """&amp;C178&amp;B178</f>
+        <f>D178&amp;" """&amp;A178&amp;""" """&amp;C178&amp;B178&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5084,7 +5084,7 @@
         </is>
       </c>
       <c r="E179">
-        <f>D179&amp;" """&amp;A179&amp;""" """&amp;C179&amp;B179</f>
+        <f>D179&amp;" """&amp;A179&amp;""" """&amp;C179&amp;B179&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5110,7 +5110,7 @@
         </is>
       </c>
       <c r="E180">
-        <f>D180&amp;" """&amp;A180&amp;""" """&amp;C180&amp;B180</f>
+        <f>D180&amp;" """&amp;A180&amp;""" """&amp;C180&amp;B180&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5136,7 +5136,7 @@
         </is>
       </c>
       <c r="E181">
-        <f>D181&amp;" """&amp;A181&amp;""" """&amp;C181&amp;B181</f>
+        <f>D181&amp;" """&amp;A181&amp;""" """&amp;C181&amp;B181&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5162,7 +5162,7 @@
         </is>
       </c>
       <c r="E182">
-        <f>D182&amp;" """&amp;A182&amp;""" """&amp;C182&amp;B182</f>
+        <f>D182&amp;" """&amp;A182&amp;""" """&amp;C182&amp;B182&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5188,7 +5188,7 @@
         </is>
       </c>
       <c r="E183">
-        <f>D183&amp;" """&amp;A183&amp;""" """&amp;C183&amp;B183</f>
+        <f>D183&amp;" """&amp;A183&amp;""" """&amp;C183&amp;B183&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5214,7 +5214,7 @@
         </is>
       </c>
       <c r="E184">
-        <f>D184&amp;" """&amp;A184&amp;""" """&amp;C184&amp;B184</f>
+        <f>D184&amp;" """&amp;A184&amp;""" """&amp;C184&amp;B184&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5240,7 +5240,7 @@
         </is>
       </c>
       <c r="E185">
-        <f>D185&amp;" """&amp;A185&amp;""" """&amp;C185&amp;B185</f>
+        <f>D185&amp;" """&amp;A185&amp;""" """&amp;C185&amp;B185&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5266,7 +5266,7 @@
         </is>
       </c>
       <c r="E186">
-        <f>D186&amp;" """&amp;A186&amp;""" """&amp;C186&amp;B186</f>
+        <f>D186&amp;" """&amp;A186&amp;""" """&amp;C186&amp;B186&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5292,7 +5292,7 @@
         </is>
       </c>
       <c r="E187">
-        <f>D187&amp;" """&amp;A187&amp;""" """&amp;C187&amp;B187</f>
+        <f>D187&amp;" """&amp;A187&amp;""" """&amp;C187&amp;B187&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5318,7 +5318,7 @@
         </is>
       </c>
       <c r="E188">
-        <f>D188&amp;" """&amp;A188&amp;""" """&amp;C188&amp;B188</f>
+        <f>D188&amp;" """&amp;A188&amp;""" """&amp;C188&amp;B188&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5344,7 +5344,7 @@
         </is>
       </c>
       <c r="E189">
-        <f>D189&amp;" """&amp;A189&amp;""" """&amp;C189&amp;B189</f>
+        <f>D189&amp;" """&amp;A189&amp;""" """&amp;C189&amp;B189&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5370,7 +5370,7 @@
         </is>
       </c>
       <c r="E190">
-        <f>D190&amp;" """&amp;A190&amp;""" """&amp;C190&amp;B190</f>
+        <f>D190&amp;" """&amp;A190&amp;""" """&amp;C190&amp;B190&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5396,7 +5396,7 @@
         </is>
       </c>
       <c r="E191">
-        <f>D191&amp;" """&amp;A191&amp;""" """&amp;C191&amp;B191</f>
+        <f>D191&amp;" """&amp;A191&amp;""" """&amp;C191&amp;B191&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5422,7 +5422,7 @@
         </is>
       </c>
       <c r="E192">
-        <f>D192&amp;" """&amp;A192&amp;""" """&amp;C192&amp;B192</f>
+        <f>D192&amp;" """&amp;A192&amp;""" """&amp;C192&amp;B192&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5448,7 +5448,7 @@
         </is>
       </c>
       <c r="E193">
-        <f>D193&amp;" """&amp;A193&amp;""" """&amp;C193&amp;B193</f>
+        <f>D193&amp;" """&amp;A193&amp;""" """&amp;C193&amp;B193&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5474,7 +5474,7 @@
         </is>
       </c>
       <c r="E194">
-        <f>D194&amp;" """&amp;A194&amp;""" """&amp;C194&amp;B194</f>
+        <f>D194&amp;" """&amp;A194&amp;""" """&amp;C194&amp;B194&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5500,7 +5500,7 @@
         </is>
       </c>
       <c r="E195">
-        <f>D195&amp;" """&amp;A195&amp;""" """&amp;C195&amp;B195</f>
+        <f>D195&amp;" """&amp;A195&amp;""" """&amp;C195&amp;B195&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5526,7 +5526,7 @@
         </is>
       </c>
       <c r="E196">
-        <f>D196&amp;" """&amp;A196&amp;""" """&amp;C196&amp;B196</f>
+        <f>D196&amp;" """&amp;A196&amp;""" """&amp;C196&amp;B196&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5552,7 +5552,7 @@
         </is>
       </c>
       <c r="E197">
-        <f>D197&amp;" """&amp;A197&amp;""" """&amp;C197&amp;B197</f>
+        <f>D197&amp;" """&amp;A197&amp;""" """&amp;C197&amp;B197&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5578,7 +5578,7 @@
         </is>
       </c>
       <c r="E198">
-        <f>D198&amp;" """&amp;A198&amp;""" """&amp;C198&amp;B198</f>
+        <f>D198&amp;" """&amp;A198&amp;""" """&amp;C198&amp;B198&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5604,7 +5604,7 @@
         </is>
       </c>
       <c r="E199">
-        <f>D199&amp;" """&amp;A199&amp;""" """&amp;C199&amp;B199</f>
+        <f>D199&amp;" """&amp;A199&amp;""" """&amp;C199&amp;B199&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5630,7 +5630,7 @@
         </is>
       </c>
       <c r="E200">
-        <f>D200&amp;" """&amp;A200&amp;""" """&amp;C200&amp;B200</f>
+        <f>D200&amp;" """&amp;A200&amp;""" """&amp;C200&amp;B200&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5656,7 +5656,7 @@
         </is>
       </c>
       <c r="E201">
-        <f>D201&amp;" """&amp;A201&amp;""" """&amp;C201&amp;B201</f>
+        <f>D201&amp;" """&amp;A201&amp;""" """&amp;C201&amp;B201&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5682,7 +5682,7 @@
         </is>
       </c>
       <c r="E202">
-        <f>D202&amp;" """&amp;A202&amp;""" """&amp;C202&amp;B202</f>
+        <f>D202&amp;" """&amp;A202&amp;""" """&amp;C202&amp;B202&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5708,7 +5708,7 @@
         </is>
       </c>
       <c r="E203">
-        <f>D203&amp;" """&amp;A203&amp;""" """&amp;C203&amp;B203</f>
+        <f>D203&amp;" """&amp;A203&amp;""" """&amp;C203&amp;B203&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5734,7 +5734,7 @@
         </is>
       </c>
       <c r="E204">
-        <f>D204&amp;" """&amp;A204&amp;""" """&amp;C204&amp;B204</f>
+        <f>D204&amp;" """&amp;A204&amp;""" """&amp;C204&amp;B204&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5760,7 +5760,7 @@
         </is>
       </c>
       <c r="E205">
-        <f>D205&amp;" """&amp;A205&amp;""" """&amp;C205&amp;B205</f>
+        <f>D205&amp;" """&amp;A205&amp;""" """&amp;C205&amp;B205&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5786,7 +5786,7 @@
         </is>
       </c>
       <c r="E206">
-        <f>D206&amp;" """&amp;A206&amp;""" """&amp;C206&amp;B206</f>
+        <f>D206&amp;" """&amp;A206&amp;""" """&amp;C206&amp;B206&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5812,7 +5812,7 @@
         </is>
       </c>
       <c r="E207">
-        <f>D207&amp;" """&amp;A207&amp;""" """&amp;C207&amp;B207</f>
+        <f>D207&amp;" """&amp;A207&amp;""" """&amp;C207&amp;B207&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5838,7 +5838,7 @@
         </is>
       </c>
       <c r="E208">
-        <f>D208&amp;" """&amp;A208&amp;""" """&amp;C208&amp;B208</f>
+        <f>D208&amp;" """&amp;A208&amp;""" """&amp;C208&amp;B208&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5864,7 +5864,7 @@
         </is>
       </c>
       <c r="E209">
-        <f>D209&amp;" """&amp;A209&amp;""" """&amp;C209&amp;B209</f>
+        <f>D209&amp;" """&amp;A209&amp;""" """&amp;C209&amp;B209&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5890,7 +5890,7 @@
         </is>
       </c>
       <c r="E210">
-        <f>D210&amp;" """&amp;A210&amp;""" """&amp;C210&amp;B210</f>
+        <f>D210&amp;" """&amp;A210&amp;""" """&amp;C210&amp;B210&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5916,7 +5916,7 @@
         </is>
       </c>
       <c r="E211">
-        <f>D211&amp;" """&amp;A211&amp;""" """&amp;C211&amp;B211</f>
+        <f>D211&amp;" """&amp;A211&amp;""" """&amp;C211&amp;B211&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5942,7 +5942,7 @@
         </is>
       </c>
       <c r="E212">
-        <f>D212&amp;" """&amp;A212&amp;""" """&amp;C212&amp;B212</f>
+        <f>D212&amp;" """&amp;A212&amp;""" """&amp;C212&amp;B212&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5968,7 +5968,7 @@
         </is>
       </c>
       <c r="E213">
-        <f>D213&amp;" """&amp;A213&amp;""" """&amp;C213&amp;B213</f>
+        <f>D213&amp;" """&amp;A213&amp;""" """&amp;C213&amp;B213&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -5994,7 +5994,7 @@
         </is>
       </c>
       <c r="E214">
-        <f>D214&amp;" """&amp;A214&amp;""" """&amp;C214&amp;B214</f>
+        <f>D214&amp;" """&amp;A214&amp;""" """&amp;C214&amp;B214&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6020,7 +6020,7 @@
         </is>
       </c>
       <c r="E215">
-        <f>D215&amp;" """&amp;A215&amp;""" """&amp;C215&amp;B215</f>
+        <f>D215&amp;" """&amp;A215&amp;""" """&amp;C215&amp;B215&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6046,7 +6046,7 @@
         </is>
       </c>
       <c r="E216">
-        <f>D216&amp;" """&amp;A216&amp;""" """&amp;C216&amp;B216</f>
+        <f>D216&amp;" """&amp;A216&amp;""" """&amp;C216&amp;B216&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6072,7 +6072,7 @@
         </is>
       </c>
       <c r="E217">
-        <f>D217&amp;" """&amp;A217&amp;""" """&amp;C217&amp;B217</f>
+        <f>D217&amp;" """&amp;A217&amp;""" """&amp;C217&amp;B217&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6098,7 +6098,7 @@
         </is>
       </c>
       <c r="E218">
-        <f>D218&amp;" """&amp;A218&amp;""" """&amp;C218&amp;B218</f>
+        <f>D218&amp;" """&amp;A218&amp;""" """&amp;C218&amp;B218&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6124,7 +6124,7 @@
         </is>
       </c>
       <c r="E219">
-        <f>D219&amp;" """&amp;A219&amp;""" """&amp;C219&amp;B219</f>
+        <f>D219&amp;" """&amp;A219&amp;""" """&amp;C219&amp;B219&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6150,7 +6150,7 @@
         </is>
       </c>
       <c r="E220">
-        <f>D220&amp;" """&amp;A220&amp;""" """&amp;C220&amp;B220</f>
+        <f>D220&amp;" """&amp;A220&amp;""" """&amp;C220&amp;B220&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6176,7 +6176,7 @@
         </is>
       </c>
       <c r="E221">
-        <f>D221&amp;" """&amp;A221&amp;""" """&amp;C221&amp;B221</f>
+        <f>D221&amp;" """&amp;A221&amp;""" """&amp;C221&amp;B221&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6202,7 +6202,7 @@
         </is>
       </c>
       <c r="E222">
-        <f>D222&amp;" """&amp;A222&amp;""" """&amp;C222&amp;B222</f>
+        <f>D222&amp;" """&amp;A222&amp;""" """&amp;C222&amp;B222&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6228,7 +6228,7 @@
         </is>
       </c>
       <c r="E223">
-        <f>D223&amp;" """&amp;A223&amp;""" """&amp;C223&amp;B223</f>
+        <f>D223&amp;" """&amp;A223&amp;""" """&amp;C223&amp;B223&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6254,7 +6254,7 @@
         </is>
       </c>
       <c r="E224">
-        <f>D224&amp;" """&amp;A224&amp;""" """&amp;C224&amp;B224</f>
+        <f>D224&amp;" """&amp;A224&amp;""" """&amp;C224&amp;B224&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6280,7 +6280,7 @@
         </is>
       </c>
       <c r="E225">
-        <f>D225&amp;" """&amp;A225&amp;""" """&amp;C225&amp;B225</f>
+        <f>D225&amp;" """&amp;A225&amp;""" """&amp;C225&amp;B225&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6306,7 +6306,7 @@
         </is>
       </c>
       <c r="E226">
-        <f>D226&amp;" """&amp;A226&amp;""" """&amp;C226&amp;B226</f>
+        <f>D226&amp;" """&amp;A226&amp;""" """&amp;C226&amp;B226&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6332,7 +6332,7 @@
         </is>
       </c>
       <c r="E227">
-        <f>D227&amp;" """&amp;A227&amp;""" """&amp;C227&amp;B227</f>
+        <f>D227&amp;" """&amp;A227&amp;""" """&amp;C227&amp;B227&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6358,7 +6358,7 @@
         </is>
       </c>
       <c r="E228">
-        <f>D228&amp;" """&amp;A228&amp;""" """&amp;C228&amp;B228</f>
+        <f>D228&amp;" """&amp;A228&amp;""" """&amp;C228&amp;B228&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6384,7 +6384,7 @@
         </is>
       </c>
       <c r="E229">
-        <f>D229&amp;" """&amp;A229&amp;""" """&amp;C229&amp;B229</f>
+        <f>D229&amp;" """&amp;A229&amp;""" """&amp;C229&amp;B229&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6410,7 +6410,7 @@
         </is>
       </c>
       <c r="E230">
-        <f>D230&amp;" """&amp;A230&amp;""" """&amp;C230&amp;B230</f>
+        <f>D230&amp;" """&amp;A230&amp;""" """&amp;C230&amp;B230&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6436,7 +6436,7 @@
         </is>
       </c>
       <c r="E231">
-        <f>D231&amp;" """&amp;A231&amp;""" """&amp;C231&amp;B231</f>
+        <f>D231&amp;" """&amp;A231&amp;""" """&amp;C231&amp;B231&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6462,7 +6462,7 @@
         </is>
       </c>
       <c r="E232">
-        <f>D232&amp;" """&amp;A232&amp;""" """&amp;C232&amp;B232</f>
+        <f>D232&amp;" """&amp;A232&amp;""" """&amp;C232&amp;B232&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6488,7 +6488,7 @@
         </is>
       </c>
       <c r="E233">
-        <f>D233&amp;" """&amp;A233&amp;""" """&amp;C233&amp;B233</f>
+        <f>D233&amp;" """&amp;A233&amp;""" """&amp;C233&amp;B233&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6514,7 +6514,7 @@
         </is>
       </c>
       <c r="E234">
-        <f>D234&amp;" """&amp;A234&amp;""" """&amp;C234&amp;B234</f>
+        <f>D234&amp;" """&amp;A234&amp;""" """&amp;C234&amp;B234&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6540,7 +6540,7 @@
         </is>
       </c>
       <c r="E235">
-        <f>D235&amp;" """&amp;A235&amp;""" """&amp;C235&amp;B235</f>
+        <f>D235&amp;" """&amp;A235&amp;""" """&amp;C235&amp;B235&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6566,7 +6566,7 @@
         </is>
       </c>
       <c r="E236">
-        <f>D236&amp;" """&amp;A236&amp;""" """&amp;C236&amp;B236</f>
+        <f>D236&amp;" """&amp;A236&amp;""" """&amp;C236&amp;B236&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6592,7 +6592,7 @@
         </is>
       </c>
       <c r="E237">
-        <f>D237&amp;" """&amp;A237&amp;""" """&amp;C237&amp;B237</f>
+        <f>D237&amp;" """&amp;A237&amp;""" """&amp;C237&amp;B237&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6618,7 +6618,7 @@
         </is>
       </c>
       <c r="E238">
-        <f>D238&amp;" """&amp;A238&amp;""" """&amp;C238&amp;B238</f>
+        <f>D238&amp;" """&amp;A238&amp;""" """&amp;C238&amp;B238&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6644,7 +6644,7 @@
         </is>
       </c>
       <c r="E239">
-        <f>D239&amp;" """&amp;A239&amp;""" """&amp;C239&amp;B239</f>
+        <f>D239&amp;" """&amp;A239&amp;""" """&amp;C239&amp;B239&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6670,7 +6670,7 @@
         </is>
       </c>
       <c r="E240">
-        <f>D240&amp;" """&amp;A240&amp;""" """&amp;C240&amp;B240</f>
+        <f>D240&amp;" """&amp;A240&amp;""" """&amp;C240&amp;B240&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6696,7 +6696,7 @@
         </is>
       </c>
       <c r="E241">
-        <f>D241&amp;" """&amp;A241&amp;""" """&amp;C241&amp;B241</f>
+        <f>D241&amp;" """&amp;A241&amp;""" """&amp;C241&amp;B241&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6722,7 +6722,7 @@
         </is>
       </c>
       <c r="E242">
-        <f>D242&amp;" """&amp;A242&amp;""" """&amp;C242&amp;B242</f>
+        <f>D242&amp;" """&amp;A242&amp;""" """&amp;C242&amp;B242&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6748,7 +6748,7 @@
         </is>
       </c>
       <c r="E243">
-        <f>D243&amp;" """&amp;A243&amp;""" """&amp;C243&amp;B243</f>
+        <f>D243&amp;" """&amp;A243&amp;""" """&amp;C243&amp;B243&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6774,7 +6774,7 @@
         </is>
       </c>
       <c r="E244">
-        <f>D244&amp;" """&amp;A244&amp;""" """&amp;C244&amp;B244</f>
+        <f>D244&amp;" """&amp;A244&amp;""" """&amp;C244&amp;B244&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6800,7 +6800,7 @@
         </is>
       </c>
       <c r="E245">
-        <f>D245&amp;" """&amp;A245&amp;""" """&amp;C245&amp;B245</f>
+        <f>D245&amp;" """&amp;A245&amp;""" """&amp;C245&amp;B245&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6826,7 +6826,7 @@
         </is>
       </c>
       <c r="E246">
-        <f>D246&amp;" """&amp;A246&amp;""" """&amp;C246&amp;B246</f>
+        <f>D246&amp;" """&amp;A246&amp;""" """&amp;C246&amp;B246&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6852,7 +6852,7 @@
         </is>
       </c>
       <c r="E247">
-        <f>D247&amp;" """&amp;A247&amp;""" """&amp;C247&amp;B247</f>
+        <f>D247&amp;" """&amp;A247&amp;""" """&amp;C247&amp;B247&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6878,7 +6878,7 @@
         </is>
       </c>
       <c r="E248">
-        <f>D248&amp;" """&amp;A248&amp;""" """&amp;C248&amp;B248</f>
+        <f>D248&amp;" """&amp;A248&amp;""" """&amp;C248&amp;B248&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6904,7 +6904,7 @@
         </is>
       </c>
       <c r="E249">
-        <f>D249&amp;" """&amp;A249&amp;""" """&amp;C249&amp;B249</f>
+        <f>D249&amp;" """&amp;A249&amp;""" """&amp;C249&amp;B249&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6930,7 +6930,7 @@
         </is>
       </c>
       <c r="E250">
-        <f>D250&amp;" """&amp;A250&amp;""" """&amp;C250&amp;B250</f>
+        <f>D250&amp;" """&amp;A250&amp;""" """&amp;C250&amp;B250&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6956,7 +6956,7 @@
         </is>
       </c>
       <c r="E251">
-        <f>D251&amp;" """&amp;A251&amp;""" """&amp;C251&amp;B251</f>
+        <f>D251&amp;" """&amp;A251&amp;""" """&amp;C251&amp;B251&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -6982,7 +6982,7 @@
         </is>
       </c>
       <c r="E252">
-        <f>D252&amp;" """&amp;A252&amp;""" """&amp;C252&amp;B252</f>
+        <f>D252&amp;" """&amp;A252&amp;""" """&amp;C252&amp;B252&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7008,7 +7008,7 @@
         </is>
       </c>
       <c r="E253">
-        <f>D253&amp;" """&amp;A253&amp;""" """&amp;C253&amp;B253</f>
+        <f>D253&amp;" """&amp;A253&amp;""" """&amp;C253&amp;B253&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7034,7 +7034,7 @@
         </is>
       </c>
       <c r="E254">
-        <f>D254&amp;" """&amp;A254&amp;""" """&amp;C254&amp;B254</f>
+        <f>D254&amp;" """&amp;A254&amp;""" """&amp;C254&amp;B254&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7060,7 +7060,7 @@
         </is>
       </c>
       <c r="E255">
-        <f>D255&amp;" """&amp;A255&amp;""" """&amp;C255&amp;B255</f>
+        <f>D255&amp;" """&amp;A255&amp;""" """&amp;C255&amp;B255&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7086,7 +7086,7 @@
         </is>
       </c>
       <c r="E256">
-        <f>D256&amp;" """&amp;A256&amp;""" """&amp;C256&amp;B256</f>
+        <f>D256&amp;" """&amp;A256&amp;""" """&amp;C256&amp;B256&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7112,7 +7112,7 @@
         </is>
       </c>
       <c r="E257">
-        <f>D257&amp;" """&amp;A257&amp;""" """&amp;C257&amp;B257</f>
+        <f>D257&amp;" """&amp;A257&amp;""" """&amp;C257&amp;B257&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7138,7 +7138,7 @@
         </is>
       </c>
       <c r="E258">
-        <f>D258&amp;" """&amp;A258&amp;""" """&amp;C258&amp;B258</f>
+        <f>D258&amp;" """&amp;A258&amp;""" """&amp;C258&amp;B258&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7164,7 +7164,7 @@
         </is>
       </c>
       <c r="E259">
-        <f>D259&amp;" """&amp;A259&amp;""" """&amp;C259&amp;B259</f>
+        <f>D259&amp;" """&amp;A259&amp;""" """&amp;C259&amp;B259&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7190,7 +7190,7 @@
         </is>
       </c>
       <c r="E260">
-        <f>D260&amp;" """&amp;A260&amp;""" """&amp;C260&amp;B260</f>
+        <f>D260&amp;" """&amp;A260&amp;""" """&amp;C260&amp;B260&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7216,7 +7216,7 @@
         </is>
       </c>
       <c r="E261">
-        <f>D261&amp;" """&amp;A261&amp;""" """&amp;C261&amp;B261</f>
+        <f>D261&amp;" """&amp;A261&amp;""" """&amp;C261&amp;B261&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7242,7 +7242,7 @@
         </is>
       </c>
       <c r="E262">
-        <f>D262&amp;" """&amp;A262&amp;""" """&amp;C262&amp;B262</f>
+        <f>D262&amp;" """&amp;A262&amp;""" """&amp;C262&amp;B262&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7268,7 +7268,7 @@
         </is>
       </c>
       <c r="E263">
-        <f>D263&amp;" """&amp;A263&amp;""" """&amp;C263&amp;B263</f>
+        <f>D263&amp;" """&amp;A263&amp;""" """&amp;C263&amp;B263&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7294,7 +7294,7 @@
         </is>
       </c>
       <c r="E264">
-        <f>D264&amp;" """&amp;A264&amp;""" """&amp;C264&amp;B264</f>
+        <f>D264&amp;" """&amp;A264&amp;""" """&amp;C264&amp;B264&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7320,7 +7320,7 @@
         </is>
       </c>
       <c r="E265">
-        <f>D265&amp;" """&amp;A265&amp;""" """&amp;C265&amp;B265</f>
+        <f>D265&amp;" """&amp;A265&amp;""" """&amp;C265&amp;B265&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7346,7 +7346,7 @@
         </is>
       </c>
       <c r="E266">
-        <f>D266&amp;" """&amp;A266&amp;""" """&amp;C266&amp;B266</f>
+        <f>D266&amp;" """&amp;A266&amp;""" """&amp;C266&amp;B266&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7372,7 +7372,7 @@
         </is>
       </c>
       <c r="E267">
-        <f>D267&amp;" """&amp;A267&amp;""" """&amp;C267&amp;B267</f>
+        <f>D267&amp;" """&amp;A267&amp;""" """&amp;C267&amp;B267&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7398,7 +7398,7 @@
         </is>
       </c>
       <c r="E268">
-        <f>D268&amp;" """&amp;A268&amp;""" """&amp;C268&amp;B268</f>
+        <f>D268&amp;" """&amp;A268&amp;""" """&amp;C268&amp;B268&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7424,7 +7424,7 @@
         </is>
       </c>
       <c r="E269">
-        <f>D269&amp;" """&amp;A269&amp;""" """&amp;C269&amp;B269</f>
+        <f>D269&amp;" """&amp;A269&amp;""" """&amp;C269&amp;B269&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7450,7 +7450,7 @@
         </is>
       </c>
       <c r="E270">
-        <f>D270&amp;" """&amp;A270&amp;""" """&amp;C270&amp;B270</f>
+        <f>D270&amp;" """&amp;A270&amp;""" """&amp;C270&amp;B270&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7476,7 +7476,7 @@
         </is>
       </c>
       <c r="E271">
-        <f>D271&amp;" """&amp;A271&amp;""" """&amp;C271&amp;B271</f>
+        <f>D271&amp;" """&amp;A271&amp;""" """&amp;C271&amp;B271&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7502,7 +7502,7 @@
         </is>
       </c>
       <c r="E272">
-        <f>D272&amp;" """&amp;A272&amp;""" """&amp;C272&amp;B272</f>
+        <f>D272&amp;" """&amp;A272&amp;""" """&amp;C272&amp;B272&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7528,7 +7528,7 @@
         </is>
       </c>
       <c r="E273">
-        <f>D273&amp;" """&amp;A273&amp;""" """&amp;C273&amp;B273</f>
+        <f>D273&amp;" """&amp;A273&amp;""" """&amp;C273&amp;B273&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7554,7 +7554,7 @@
         </is>
       </c>
       <c r="E274">
-        <f>D274&amp;" """&amp;A274&amp;""" """&amp;C274&amp;B274</f>
+        <f>D274&amp;" """&amp;A274&amp;""" """&amp;C274&amp;B274&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7580,7 +7580,7 @@
         </is>
       </c>
       <c r="E275">
-        <f>D275&amp;" """&amp;A275&amp;""" """&amp;C275&amp;B275</f>
+        <f>D275&amp;" """&amp;A275&amp;""" """&amp;C275&amp;B275&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7606,7 +7606,7 @@
         </is>
       </c>
       <c r="E276">
-        <f>D276&amp;" """&amp;A276&amp;""" """&amp;C276&amp;B276</f>
+        <f>D276&amp;" """&amp;A276&amp;""" """&amp;C276&amp;B276&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7632,7 +7632,7 @@
         </is>
       </c>
       <c r="E277">
-        <f>D277&amp;" """&amp;A277&amp;""" """&amp;C277&amp;B277</f>
+        <f>D277&amp;" """&amp;A277&amp;""" """&amp;C277&amp;B277&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7658,7 +7658,7 @@
         </is>
       </c>
       <c r="E278">
-        <f>D278&amp;" """&amp;A278&amp;""" """&amp;C278&amp;B278</f>
+        <f>D278&amp;" """&amp;A278&amp;""" """&amp;C278&amp;B278&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7684,7 +7684,7 @@
         </is>
       </c>
       <c r="E279">
-        <f>D279&amp;" """&amp;A279&amp;""" """&amp;C279&amp;B279</f>
+        <f>D279&amp;" """&amp;A279&amp;""" """&amp;C279&amp;B279&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7710,7 +7710,7 @@
         </is>
       </c>
       <c r="E280">
-        <f>D280&amp;" """&amp;A280&amp;""" """&amp;C280&amp;B280</f>
+        <f>D280&amp;" """&amp;A280&amp;""" """&amp;C280&amp;B280&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7736,7 +7736,7 @@
         </is>
       </c>
       <c r="E281">
-        <f>D281&amp;" """&amp;A281&amp;""" """&amp;C281&amp;B281</f>
+        <f>D281&amp;" """&amp;A281&amp;""" """&amp;C281&amp;B281&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7762,7 +7762,7 @@
         </is>
       </c>
       <c r="E282">
-        <f>D282&amp;" """&amp;A282&amp;""" """&amp;C282&amp;B282</f>
+        <f>D282&amp;" """&amp;A282&amp;""" """&amp;C282&amp;B282&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7788,7 +7788,7 @@
         </is>
       </c>
       <c r="E283">
-        <f>D283&amp;" """&amp;A283&amp;""" """&amp;C283&amp;B283</f>
+        <f>D283&amp;" """&amp;A283&amp;""" """&amp;C283&amp;B283&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7814,7 +7814,7 @@
         </is>
       </c>
       <c r="E284">
-        <f>D284&amp;" """&amp;A284&amp;""" """&amp;C284&amp;B284</f>
+        <f>D284&amp;" """&amp;A284&amp;""" """&amp;C284&amp;B284&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7840,7 +7840,7 @@
         </is>
       </c>
       <c r="E285">
-        <f>D285&amp;" """&amp;A285&amp;""" """&amp;C285&amp;B285</f>
+        <f>D285&amp;" """&amp;A285&amp;""" """&amp;C285&amp;B285&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7866,7 +7866,7 @@
         </is>
       </c>
       <c r="E286">
-        <f>D286&amp;" """&amp;A286&amp;""" """&amp;C286&amp;B286</f>
+        <f>D286&amp;" """&amp;A286&amp;""" """&amp;C286&amp;B286&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7892,7 +7892,7 @@
         </is>
       </c>
       <c r="E287">
-        <f>D287&amp;" """&amp;A287&amp;""" """&amp;C287&amp;B287</f>
+        <f>D287&amp;" """&amp;A287&amp;""" """&amp;C287&amp;B287&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7918,7 +7918,7 @@
         </is>
       </c>
       <c r="E288">
-        <f>D288&amp;" """&amp;A288&amp;""" """&amp;C288&amp;B288</f>
+        <f>D288&amp;" """&amp;A288&amp;""" """&amp;C288&amp;B288&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7944,7 +7944,7 @@
         </is>
       </c>
       <c r="E289">
-        <f>D289&amp;" """&amp;A289&amp;""" """&amp;C289&amp;B289</f>
+        <f>D289&amp;" """&amp;A289&amp;""" """&amp;C289&amp;B289&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7970,7 +7970,7 @@
         </is>
       </c>
       <c r="E290">
-        <f>D290&amp;" """&amp;A290&amp;""" """&amp;C290&amp;B290</f>
+        <f>D290&amp;" """&amp;A290&amp;""" """&amp;C290&amp;B290&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -7996,7 +7996,7 @@
         </is>
       </c>
       <c r="E291">
-        <f>D291&amp;" """&amp;A291&amp;""" """&amp;C291&amp;B291</f>
+        <f>D291&amp;" """&amp;A291&amp;""" """&amp;C291&amp;B291&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8022,7 +8022,7 @@
         </is>
       </c>
       <c r="E292">
-        <f>D292&amp;" """&amp;A292&amp;""" """&amp;C292&amp;B292</f>
+        <f>D292&amp;" """&amp;A292&amp;""" """&amp;C292&amp;B292&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8048,7 +8048,7 @@
         </is>
       </c>
       <c r="E293">
-        <f>D293&amp;" """&amp;A293&amp;""" """&amp;C293&amp;B293</f>
+        <f>D293&amp;" """&amp;A293&amp;""" """&amp;C293&amp;B293&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8074,7 +8074,7 @@
         </is>
       </c>
       <c r="E294">
-        <f>D294&amp;" """&amp;A294&amp;""" """&amp;C294&amp;B294</f>
+        <f>D294&amp;" """&amp;A294&amp;""" """&amp;C294&amp;B294&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8100,7 +8100,7 @@
         </is>
       </c>
       <c r="E295">
-        <f>D295&amp;" """&amp;A295&amp;""" """&amp;C295&amp;B295</f>
+        <f>D295&amp;" """&amp;A295&amp;""" """&amp;C295&amp;B295&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8126,7 +8126,7 @@
         </is>
       </c>
       <c r="E296">
-        <f>D296&amp;" """&amp;A296&amp;""" """&amp;C296&amp;B296</f>
+        <f>D296&amp;" """&amp;A296&amp;""" """&amp;C296&amp;B296&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8152,7 +8152,7 @@
         </is>
       </c>
       <c r="E297">
-        <f>D297&amp;" """&amp;A297&amp;""" """&amp;C297&amp;B297</f>
+        <f>D297&amp;" """&amp;A297&amp;""" """&amp;C297&amp;B297&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8178,7 +8178,7 @@
         </is>
       </c>
       <c r="E298">
-        <f>D298&amp;" """&amp;A298&amp;""" """&amp;C298&amp;B298</f>
+        <f>D298&amp;" """&amp;A298&amp;""" """&amp;C298&amp;B298&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8204,7 +8204,7 @@
         </is>
       </c>
       <c r="E299">
-        <f>D299&amp;" """&amp;A299&amp;""" """&amp;C299&amp;B299</f>
+        <f>D299&amp;" """&amp;A299&amp;""" """&amp;C299&amp;B299&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8230,7 +8230,7 @@
         </is>
       </c>
       <c r="E300">
-        <f>D300&amp;" """&amp;A300&amp;""" """&amp;C300&amp;B300</f>
+        <f>D300&amp;" """&amp;A300&amp;""" """&amp;C300&amp;B300&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8256,7 +8256,7 @@
         </is>
       </c>
       <c r="E301">
-        <f>D301&amp;" """&amp;A301&amp;""" """&amp;C301&amp;B301</f>
+        <f>D301&amp;" """&amp;A301&amp;""" """&amp;C301&amp;B301&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8282,7 +8282,7 @@
         </is>
       </c>
       <c r="E302">
-        <f>D302&amp;" """&amp;A302&amp;""" """&amp;C302&amp;B302</f>
+        <f>D302&amp;" """&amp;A302&amp;""" """&amp;C302&amp;B302&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8308,7 +8308,7 @@
         </is>
       </c>
       <c r="E303">
-        <f>D303&amp;" """&amp;A303&amp;""" """&amp;C303&amp;B303</f>
+        <f>D303&amp;" """&amp;A303&amp;""" """&amp;C303&amp;B303&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8334,7 +8334,7 @@
         </is>
       </c>
       <c r="E304">
-        <f>D304&amp;" """&amp;A304&amp;""" """&amp;C304&amp;B304</f>
+        <f>D304&amp;" """&amp;A304&amp;""" """&amp;C304&amp;B304&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8360,7 +8360,7 @@
         </is>
       </c>
       <c r="E305">
-        <f>D305&amp;" """&amp;A305&amp;""" """&amp;C305&amp;B305</f>
+        <f>D305&amp;" """&amp;A305&amp;""" """&amp;C305&amp;B305&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8386,7 +8386,7 @@
         </is>
       </c>
       <c r="E306">
-        <f>D306&amp;" """&amp;A306&amp;""" """&amp;C306&amp;B306</f>
+        <f>D306&amp;" """&amp;A306&amp;""" """&amp;C306&amp;B306&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8412,7 +8412,7 @@
         </is>
       </c>
       <c r="E307">
-        <f>D307&amp;" """&amp;A307&amp;""" """&amp;C307&amp;B307</f>
+        <f>D307&amp;" """&amp;A307&amp;""" """&amp;C307&amp;B307&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8438,7 +8438,7 @@
         </is>
       </c>
       <c r="E308">
-        <f>D308&amp;" """&amp;A308&amp;""" """&amp;C308&amp;B308</f>
+        <f>D308&amp;" """&amp;A308&amp;""" """&amp;C308&amp;B308&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8464,7 +8464,7 @@
         </is>
       </c>
       <c r="E309">
-        <f>D309&amp;" """&amp;A309&amp;""" """&amp;C309&amp;B309</f>
+        <f>D309&amp;" """&amp;A309&amp;""" """&amp;C309&amp;B309&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8490,7 +8490,7 @@
         </is>
       </c>
       <c r="E310">
-        <f>D310&amp;" """&amp;A310&amp;""" """&amp;C310&amp;B310</f>
+        <f>D310&amp;" """&amp;A310&amp;""" """&amp;C310&amp;B310&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8516,7 +8516,7 @@
         </is>
       </c>
       <c r="E311">
-        <f>D311&amp;" """&amp;A311&amp;""" """&amp;C311&amp;B311</f>
+        <f>D311&amp;" """&amp;A311&amp;""" """&amp;C311&amp;B311&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8542,7 +8542,7 @@
         </is>
       </c>
       <c r="E312">
-        <f>D312&amp;" """&amp;A312&amp;""" """&amp;C312&amp;B312</f>
+        <f>D312&amp;" """&amp;A312&amp;""" """&amp;C312&amp;B312&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8568,7 +8568,7 @@
         </is>
       </c>
       <c r="E313">
-        <f>D313&amp;" """&amp;A313&amp;""" """&amp;C313&amp;B313</f>
+        <f>D313&amp;" """&amp;A313&amp;""" """&amp;C313&amp;B313&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8594,7 +8594,7 @@
         </is>
       </c>
       <c r="E314">
-        <f>D314&amp;" """&amp;A314&amp;""" """&amp;C314&amp;B314</f>
+        <f>D314&amp;" """&amp;A314&amp;""" """&amp;C314&amp;B314&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8620,7 +8620,7 @@
         </is>
       </c>
       <c r="E315">
-        <f>D315&amp;" """&amp;A315&amp;""" """&amp;C315&amp;B315</f>
+        <f>D315&amp;" """&amp;A315&amp;""" """&amp;C315&amp;B315&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8646,7 +8646,7 @@
         </is>
       </c>
       <c r="E316">
-        <f>D316&amp;" """&amp;A316&amp;""" """&amp;C316&amp;B316</f>
+        <f>D316&amp;" """&amp;A316&amp;""" """&amp;C316&amp;B316&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8672,7 +8672,7 @@
         </is>
       </c>
       <c r="E317">
-        <f>D317&amp;" """&amp;A317&amp;""" """&amp;C317&amp;B317</f>
+        <f>D317&amp;" """&amp;A317&amp;""" """&amp;C317&amp;B317&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8698,7 +8698,7 @@
         </is>
       </c>
       <c r="E318">
-        <f>D318&amp;" """&amp;A318&amp;""" """&amp;C318&amp;B318</f>
+        <f>D318&amp;" """&amp;A318&amp;""" """&amp;C318&amp;B318&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8724,7 +8724,7 @@
         </is>
       </c>
       <c r="E319">
-        <f>D319&amp;" """&amp;A319&amp;""" """&amp;C319&amp;B319</f>
+        <f>D319&amp;" """&amp;A319&amp;""" """&amp;C319&amp;B319&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8750,7 +8750,7 @@
         </is>
       </c>
       <c r="E320">
-        <f>D320&amp;" """&amp;A320&amp;""" """&amp;C320&amp;B320</f>
+        <f>D320&amp;" """&amp;A320&amp;""" """&amp;C320&amp;B320&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8776,7 +8776,7 @@
         </is>
       </c>
       <c r="E321">
-        <f>D321&amp;" """&amp;A321&amp;""" """&amp;C321&amp;B321</f>
+        <f>D321&amp;" """&amp;A321&amp;""" """&amp;C321&amp;B321&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8802,7 +8802,7 @@
         </is>
       </c>
       <c r="E322">
-        <f>D322&amp;" """&amp;A322&amp;""" """&amp;C322&amp;B322</f>
+        <f>D322&amp;" """&amp;A322&amp;""" """&amp;C322&amp;B322&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8828,7 +8828,7 @@
         </is>
       </c>
       <c r="E323">
-        <f>D323&amp;" """&amp;A323&amp;""" """&amp;C323&amp;B323</f>
+        <f>D323&amp;" """&amp;A323&amp;""" """&amp;C323&amp;B323&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8854,7 +8854,7 @@
         </is>
       </c>
       <c r="E324">
-        <f>D324&amp;" """&amp;A324&amp;""" """&amp;C324&amp;B324</f>
+        <f>D324&amp;" """&amp;A324&amp;""" """&amp;C324&amp;B324&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8880,7 +8880,7 @@
         </is>
       </c>
       <c r="E325">
-        <f>D325&amp;" """&amp;A325&amp;""" """&amp;C325&amp;B325</f>
+        <f>D325&amp;" """&amp;A325&amp;""" """&amp;C325&amp;B325&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8906,7 +8906,7 @@
         </is>
       </c>
       <c r="E326">
-        <f>D326&amp;" """&amp;A326&amp;""" """&amp;C326&amp;B326</f>
+        <f>D326&amp;" """&amp;A326&amp;""" """&amp;C326&amp;B326&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8932,7 +8932,7 @@
         </is>
       </c>
       <c r="E327">
-        <f>D327&amp;" """&amp;A327&amp;""" """&amp;C327&amp;B327</f>
+        <f>D327&amp;" """&amp;A327&amp;""" """&amp;C327&amp;B327&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8958,7 +8958,7 @@
         </is>
       </c>
       <c r="E328">
-        <f>D328&amp;" """&amp;A328&amp;""" """&amp;C328&amp;B328</f>
+        <f>D328&amp;" """&amp;A328&amp;""" """&amp;C328&amp;B328&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -8984,7 +8984,7 @@
         </is>
       </c>
       <c r="E329">
-        <f>D329&amp;" """&amp;A329&amp;""" """&amp;C329&amp;B329</f>
+        <f>D329&amp;" """&amp;A329&amp;""" """&amp;C329&amp;B329&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9010,7 +9010,7 @@
         </is>
       </c>
       <c r="E330">
-        <f>D330&amp;" """&amp;A330&amp;""" """&amp;C330&amp;B330</f>
+        <f>D330&amp;" """&amp;A330&amp;""" """&amp;C330&amp;B330&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9036,7 +9036,7 @@
         </is>
       </c>
       <c r="E331">
-        <f>D331&amp;" """&amp;A331&amp;""" """&amp;C331&amp;B331</f>
+        <f>D331&amp;" """&amp;A331&amp;""" """&amp;C331&amp;B331&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9062,7 +9062,7 @@
         </is>
       </c>
       <c r="E332">
-        <f>D332&amp;" """&amp;A332&amp;""" """&amp;C332&amp;B332</f>
+        <f>D332&amp;" """&amp;A332&amp;""" """&amp;C332&amp;B332&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9088,7 +9088,7 @@
         </is>
       </c>
       <c r="E333">
-        <f>D333&amp;" """&amp;A333&amp;""" """&amp;C333&amp;B333</f>
+        <f>D333&amp;" """&amp;A333&amp;""" """&amp;C333&amp;B333&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9114,7 +9114,7 @@
         </is>
       </c>
       <c r="E334">
-        <f>D334&amp;" """&amp;A334&amp;""" """&amp;C334&amp;B334</f>
+        <f>D334&amp;" """&amp;A334&amp;""" """&amp;C334&amp;B334&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9140,7 +9140,7 @@
         </is>
       </c>
       <c r="E335">
-        <f>D335&amp;" """&amp;A335&amp;""" """&amp;C335&amp;B335</f>
+        <f>D335&amp;" """&amp;A335&amp;""" """&amp;C335&amp;B335&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9166,7 +9166,7 @@
         </is>
       </c>
       <c r="E336">
-        <f>D336&amp;" """&amp;A336&amp;""" """&amp;C336&amp;B336</f>
+        <f>D336&amp;" """&amp;A336&amp;""" """&amp;C336&amp;B336&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9192,7 +9192,7 @@
         </is>
       </c>
       <c r="E337">
-        <f>D337&amp;" """&amp;A337&amp;""" """&amp;C337&amp;B337</f>
+        <f>D337&amp;" """&amp;A337&amp;""" """&amp;C337&amp;B337&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9218,7 +9218,7 @@
         </is>
       </c>
       <c r="E338">
-        <f>D338&amp;" """&amp;A338&amp;""" """&amp;C338&amp;B338</f>
+        <f>D338&amp;" """&amp;A338&amp;""" """&amp;C338&amp;B338&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9244,7 +9244,7 @@
         </is>
       </c>
       <c r="E339">
-        <f>D339&amp;" """&amp;A339&amp;""" """&amp;C339&amp;B339</f>
+        <f>D339&amp;" """&amp;A339&amp;""" """&amp;C339&amp;B339&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9270,7 +9270,7 @@
         </is>
       </c>
       <c r="E340">
-        <f>D340&amp;" """&amp;A340&amp;""" """&amp;C340&amp;B340</f>
+        <f>D340&amp;" """&amp;A340&amp;""" """&amp;C340&amp;B340&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9296,7 +9296,7 @@
         </is>
       </c>
       <c r="E341">
-        <f>D341&amp;" """&amp;A341&amp;""" """&amp;C341&amp;B341</f>
+        <f>D341&amp;" """&amp;A341&amp;""" """&amp;C341&amp;B341&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9322,7 +9322,7 @@
         </is>
       </c>
       <c r="E342">
-        <f>D342&amp;" """&amp;A342&amp;""" """&amp;C342&amp;B342</f>
+        <f>D342&amp;" """&amp;A342&amp;""" """&amp;C342&amp;B342&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9348,7 +9348,7 @@
         </is>
       </c>
       <c r="E343">
-        <f>D343&amp;" """&amp;A343&amp;""" """&amp;C343&amp;B343</f>
+        <f>D343&amp;" """&amp;A343&amp;""" """&amp;C343&amp;B343&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9374,7 +9374,7 @@
         </is>
       </c>
       <c r="E344">
-        <f>D344&amp;" """&amp;A344&amp;""" """&amp;C344&amp;B344</f>
+        <f>D344&amp;" """&amp;A344&amp;""" """&amp;C344&amp;B344&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9400,7 +9400,7 @@
         </is>
       </c>
       <c r="E345">
-        <f>D345&amp;" """&amp;A345&amp;""" """&amp;C345&amp;B345</f>
+        <f>D345&amp;" """&amp;A345&amp;""" """&amp;C345&amp;B345&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9426,7 +9426,7 @@
         </is>
       </c>
       <c r="E346">
-        <f>D346&amp;" """&amp;A346&amp;""" """&amp;C346&amp;B346</f>
+        <f>D346&amp;" """&amp;A346&amp;""" """&amp;C346&amp;B346&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9452,7 +9452,7 @@
         </is>
       </c>
       <c r="E347">
-        <f>D347&amp;" """&amp;A347&amp;""" """&amp;C347&amp;B347</f>
+        <f>D347&amp;" """&amp;A347&amp;""" """&amp;C347&amp;B347&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9478,7 +9478,7 @@
         </is>
       </c>
       <c r="E348">
-        <f>D348&amp;" """&amp;A348&amp;""" """&amp;C348&amp;B348</f>
+        <f>D348&amp;" """&amp;A348&amp;""" """&amp;C348&amp;B348&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9504,7 +9504,7 @@
         </is>
       </c>
       <c r="E349">
-        <f>D349&amp;" """&amp;A349&amp;""" """&amp;C349&amp;B349</f>
+        <f>D349&amp;" """&amp;A349&amp;""" """&amp;C349&amp;B349&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9530,7 +9530,7 @@
         </is>
       </c>
       <c r="E350">
-        <f>D350&amp;" """&amp;A350&amp;""" """&amp;C350&amp;B350</f>
+        <f>D350&amp;" """&amp;A350&amp;""" """&amp;C350&amp;B350&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9556,7 +9556,7 @@
         </is>
       </c>
       <c r="E351">
-        <f>D351&amp;" """&amp;A351&amp;""" """&amp;C351&amp;B351</f>
+        <f>D351&amp;" """&amp;A351&amp;""" """&amp;C351&amp;B351&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9582,7 +9582,7 @@
         </is>
       </c>
       <c r="E352">
-        <f>D352&amp;" """&amp;A352&amp;""" """&amp;C352&amp;B352</f>
+        <f>D352&amp;" """&amp;A352&amp;""" """&amp;C352&amp;B352&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9608,7 +9608,7 @@
         </is>
       </c>
       <c r="E353">
-        <f>D353&amp;" """&amp;A353&amp;""" """&amp;C353&amp;B353</f>
+        <f>D353&amp;" """&amp;A353&amp;""" """&amp;C353&amp;B353&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9634,7 +9634,7 @@
         </is>
       </c>
       <c r="E354">
-        <f>D354&amp;" """&amp;A354&amp;""" """&amp;C354&amp;B354</f>
+        <f>D354&amp;" """&amp;A354&amp;""" """&amp;C354&amp;B354&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9660,7 +9660,7 @@
         </is>
       </c>
       <c r="E355">
-        <f>D355&amp;" """&amp;A355&amp;""" """&amp;C355&amp;B355</f>
+        <f>D355&amp;" """&amp;A355&amp;""" """&amp;C355&amp;B355&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9686,7 +9686,7 @@
         </is>
       </c>
       <c r="E356">
-        <f>D356&amp;" """&amp;A356&amp;""" """&amp;C356&amp;B356</f>
+        <f>D356&amp;" """&amp;A356&amp;""" """&amp;C356&amp;B356&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9712,7 +9712,7 @@
         </is>
       </c>
       <c r="E357">
-        <f>D357&amp;" """&amp;A357&amp;""" """&amp;C357&amp;B357</f>
+        <f>D357&amp;" """&amp;A357&amp;""" """&amp;C357&amp;B357&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9738,7 +9738,7 @@
         </is>
       </c>
       <c r="E358">
-        <f>D358&amp;" """&amp;A358&amp;""" """&amp;C358&amp;B358</f>
+        <f>D358&amp;" """&amp;A358&amp;""" """&amp;C358&amp;B358&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9764,7 +9764,7 @@
         </is>
       </c>
       <c r="E359">
-        <f>D359&amp;" """&amp;A359&amp;""" """&amp;C359&amp;B359</f>
+        <f>D359&amp;" """&amp;A359&amp;""" """&amp;C359&amp;B359&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9790,7 +9790,7 @@
         </is>
       </c>
       <c r="E360">
-        <f>D360&amp;" """&amp;A360&amp;""" """&amp;C360&amp;B360</f>
+        <f>D360&amp;" """&amp;A360&amp;""" """&amp;C360&amp;B360&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9816,7 +9816,7 @@
         </is>
       </c>
       <c r="E361">
-        <f>D361&amp;" """&amp;A361&amp;""" """&amp;C361&amp;B361</f>
+        <f>D361&amp;" """&amp;A361&amp;""" """&amp;C361&amp;B361&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9842,7 +9842,7 @@
         </is>
       </c>
       <c r="E362">
-        <f>D362&amp;" """&amp;A362&amp;""" """&amp;C362&amp;B362</f>
+        <f>D362&amp;" """&amp;A362&amp;""" """&amp;C362&amp;B362&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9868,7 +9868,7 @@
         </is>
       </c>
       <c r="E363">
-        <f>D363&amp;" """&amp;A363&amp;""" """&amp;C363&amp;B363</f>
+        <f>D363&amp;" """&amp;A363&amp;""" """&amp;C363&amp;B363&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9894,7 +9894,7 @@
         </is>
       </c>
       <c r="E364">
-        <f>D364&amp;" """&amp;A364&amp;""" """&amp;C364&amp;B364</f>
+        <f>D364&amp;" """&amp;A364&amp;""" """&amp;C364&amp;B364&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9920,7 +9920,7 @@
         </is>
       </c>
       <c r="E365">
-        <f>D365&amp;" """&amp;A365&amp;""" """&amp;C365&amp;B365</f>
+        <f>D365&amp;" """&amp;A365&amp;""" """&amp;C365&amp;B365&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9946,7 +9946,7 @@
         </is>
       </c>
       <c r="E366">
-        <f>D366&amp;" """&amp;A366&amp;""" """&amp;C366&amp;B366</f>
+        <f>D366&amp;" """&amp;A366&amp;""" """&amp;C366&amp;B366&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9972,7 +9972,7 @@
         </is>
       </c>
       <c r="E367">
-        <f>D367&amp;" """&amp;A367&amp;""" """&amp;C367&amp;B367</f>
+        <f>D367&amp;" """&amp;A367&amp;""" """&amp;C367&amp;B367&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -9998,7 +9998,7 @@
         </is>
       </c>
       <c r="E368">
-        <f>D368&amp;" """&amp;A368&amp;""" """&amp;C368&amp;B368</f>
+        <f>D368&amp;" """&amp;A368&amp;""" """&amp;C368&amp;B368&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10024,7 +10024,7 @@
         </is>
       </c>
       <c r="E369">
-        <f>D369&amp;" """&amp;A369&amp;""" """&amp;C369&amp;B369</f>
+        <f>D369&amp;" """&amp;A369&amp;""" """&amp;C369&amp;B369&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10050,7 +10050,7 @@
         </is>
       </c>
       <c r="E370">
-        <f>D370&amp;" """&amp;A370&amp;""" """&amp;C370&amp;B370</f>
+        <f>D370&amp;" """&amp;A370&amp;""" """&amp;C370&amp;B370&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10076,7 +10076,7 @@
         </is>
       </c>
       <c r="E371">
-        <f>D371&amp;" """&amp;A371&amp;""" """&amp;C371&amp;B371</f>
+        <f>D371&amp;" """&amp;A371&amp;""" """&amp;C371&amp;B371&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10102,7 +10102,7 @@
         </is>
       </c>
       <c r="E372">
-        <f>D372&amp;" """&amp;A372&amp;""" """&amp;C372&amp;B372</f>
+        <f>D372&amp;" """&amp;A372&amp;""" """&amp;C372&amp;B372&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10128,7 +10128,7 @@
         </is>
       </c>
       <c r="E373">
-        <f>D373&amp;" """&amp;A373&amp;""" """&amp;C373&amp;B373</f>
+        <f>D373&amp;" """&amp;A373&amp;""" """&amp;C373&amp;B373&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10154,7 +10154,7 @@
         </is>
       </c>
       <c r="E374">
-        <f>D374&amp;" """&amp;A374&amp;""" """&amp;C374&amp;B374</f>
+        <f>D374&amp;" """&amp;A374&amp;""" """&amp;C374&amp;B374&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10180,7 +10180,7 @@
         </is>
       </c>
       <c r="E375">
-        <f>D375&amp;" """&amp;A375&amp;""" """&amp;C375&amp;B375</f>
+        <f>D375&amp;" """&amp;A375&amp;""" """&amp;C375&amp;B375&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10206,7 +10206,7 @@
         </is>
       </c>
       <c r="E376">
-        <f>D376&amp;" """&amp;A376&amp;""" """&amp;C376&amp;B376</f>
+        <f>D376&amp;" """&amp;A376&amp;""" """&amp;C376&amp;B376&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10232,7 +10232,7 @@
         </is>
       </c>
       <c r="E377">
-        <f>D377&amp;" """&amp;A377&amp;""" """&amp;C377&amp;B377</f>
+        <f>D377&amp;" """&amp;A377&amp;""" """&amp;C377&amp;B377&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10258,7 +10258,7 @@
         </is>
       </c>
       <c r="E378">
-        <f>D378&amp;" """&amp;A378&amp;""" """&amp;C378&amp;B378</f>
+        <f>D378&amp;" """&amp;A378&amp;""" """&amp;C378&amp;B378&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10284,7 +10284,7 @@
         </is>
       </c>
       <c r="E379">
-        <f>D379&amp;" """&amp;A379&amp;""" """&amp;C379&amp;B379</f>
+        <f>D379&amp;" """&amp;A379&amp;""" """&amp;C379&amp;B379&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10310,7 +10310,7 @@
         </is>
       </c>
       <c r="E380">
-        <f>D380&amp;" """&amp;A380&amp;""" """&amp;C380&amp;B380</f>
+        <f>D380&amp;" """&amp;A380&amp;""" """&amp;C380&amp;B380&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10336,7 +10336,7 @@
         </is>
       </c>
       <c r="E381">
-        <f>D381&amp;" """&amp;A381&amp;""" """&amp;C381&amp;B381</f>
+        <f>D381&amp;" """&amp;A381&amp;""" """&amp;C381&amp;B381&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10362,7 +10362,7 @@
         </is>
       </c>
       <c r="E382">
-        <f>D382&amp;" """&amp;A382&amp;""" """&amp;C382&amp;B382</f>
+        <f>D382&amp;" """&amp;A382&amp;""" """&amp;C382&amp;B382&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10388,7 +10388,7 @@
         </is>
       </c>
       <c r="E383">
-        <f>D383&amp;" """&amp;A383&amp;""" """&amp;C383&amp;B383</f>
+        <f>D383&amp;" """&amp;A383&amp;""" """&amp;C383&amp;B383&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10414,7 +10414,7 @@
         </is>
       </c>
       <c r="E384">
-        <f>D384&amp;" """&amp;A384&amp;""" """&amp;C384&amp;B384</f>
+        <f>D384&amp;" """&amp;A384&amp;""" """&amp;C384&amp;B384&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10440,7 +10440,7 @@
         </is>
       </c>
       <c r="E385">
-        <f>D385&amp;" """&amp;A385&amp;""" """&amp;C385&amp;B385</f>
+        <f>D385&amp;" """&amp;A385&amp;""" """&amp;C385&amp;B385&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10466,7 +10466,7 @@
         </is>
       </c>
       <c r="E386">
-        <f>D386&amp;" """&amp;A386&amp;""" """&amp;C386&amp;B386</f>
+        <f>D386&amp;" """&amp;A386&amp;""" """&amp;C386&amp;B386&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10492,7 +10492,7 @@
         </is>
       </c>
       <c r="E387">
-        <f>D387&amp;" """&amp;A387&amp;""" """&amp;C387&amp;B387</f>
+        <f>D387&amp;" """&amp;A387&amp;""" """&amp;C387&amp;B387&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10518,7 +10518,7 @@
         </is>
       </c>
       <c r="E388">
-        <f>D388&amp;" """&amp;A388&amp;""" """&amp;C388&amp;B388</f>
+        <f>D388&amp;" """&amp;A388&amp;""" """&amp;C388&amp;B388&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10544,7 +10544,7 @@
         </is>
       </c>
       <c r="E389">
-        <f>D389&amp;" """&amp;A389&amp;""" """&amp;C389&amp;B389</f>
+        <f>D389&amp;" """&amp;A389&amp;""" """&amp;C389&amp;B389&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10570,7 +10570,7 @@
         </is>
       </c>
       <c r="E390">
-        <f>D390&amp;" """&amp;A390&amp;""" """&amp;C390&amp;B390</f>
+        <f>D390&amp;" """&amp;A390&amp;""" """&amp;C390&amp;B390&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10596,7 +10596,7 @@
         </is>
       </c>
       <c r="E391">
-        <f>D391&amp;" """&amp;A391&amp;""" """&amp;C391&amp;B391</f>
+        <f>D391&amp;" """&amp;A391&amp;""" """&amp;C391&amp;B391&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10622,7 +10622,7 @@
         </is>
       </c>
       <c r="E392">
-        <f>D392&amp;" """&amp;A392&amp;""" """&amp;C392&amp;B392</f>
+        <f>D392&amp;" """&amp;A392&amp;""" """&amp;C392&amp;B392&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10648,7 +10648,7 @@
         </is>
       </c>
       <c r="E393">
-        <f>D393&amp;" """&amp;A393&amp;""" """&amp;C393&amp;B393</f>
+        <f>D393&amp;" """&amp;A393&amp;""" """&amp;C393&amp;B393&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10674,7 +10674,7 @@
         </is>
       </c>
       <c r="E394">
-        <f>D394&amp;" """&amp;A394&amp;""" """&amp;C394&amp;B394</f>
+        <f>D394&amp;" """&amp;A394&amp;""" """&amp;C394&amp;B394&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10700,7 +10700,7 @@
         </is>
       </c>
       <c r="E395">
-        <f>D395&amp;" """&amp;A395&amp;""" """&amp;C395&amp;B395</f>
+        <f>D395&amp;" """&amp;A395&amp;""" """&amp;C395&amp;B395&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10726,7 +10726,7 @@
         </is>
       </c>
       <c r="E396">
-        <f>D396&amp;" """&amp;A396&amp;""" """&amp;C396&amp;B396</f>
+        <f>D396&amp;" """&amp;A396&amp;""" """&amp;C396&amp;B396&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10752,7 +10752,7 @@
         </is>
       </c>
       <c r="E397">
-        <f>D397&amp;" """&amp;A397&amp;""" """&amp;C397&amp;B397</f>
+        <f>D397&amp;" """&amp;A397&amp;""" """&amp;C397&amp;B397&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10778,7 +10778,7 @@
         </is>
       </c>
       <c r="E398">
-        <f>D398&amp;" """&amp;A398&amp;""" """&amp;C398&amp;B398</f>
+        <f>D398&amp;" """&amp;A398&amp;""" """&amp;C398&amp;B398&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10804,7 +10804,7 @@
         </is>
       </c>
       <c r="E399">
-        <f>D399&amp;" """&amp;A399&amp;""" """&amp;C399&amp;B399</f>
+        <f>D399&amp;" """&amp;A399&amp;""" """&amp;C399&amp;B399&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10830,7 +10830,7 @@
         </is>
       </c>
       <c r="E400">
-        <f>D400&amp;" """&amp;A400&amp;""" """&amp;C400&amp;B400</f>
+        <f>D400&amp;" """&amp;A400&amp;""" """&amp;C400&amp;B400&amp;""""</f>
         <v/>
       </c>
     </row>
@@ -10856,7 +10856,7 @@
         </is>
       </c>
       <c r="E401">
-        <f>D401&amp;" """&amp;A401&amp;""" """&amp;C401&amp;B401</f>
+        <f>D401&amp;" """&amp;A401&amp;""" """&amp;C401&amp;B401&amp;""""</f>
         <v/>
       </c>
     </row>

</xml_diff>